<commit_message>
CARLA-3 1. Closed all spaces as recommended. 2. "Undetermine" is used for all variables that needs information. 3. Cancer types will be under "undetermine" because I am yet to conclude on catergories 4. There is still an error with EDU after regrouping from highest to lowest and correcting lower case in both DPEs and DD.
</commit_message>
<xml_diff>
--- a/analyst/Tracy/rmonize/data_dictionary/DD_CARLA_TRACY.xlsx
+++ b/analyst/Tracy/rmonize/data_dictionary/DD_CARLA_TRACY.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="K:\use-cases-harmonisation\use-cases-harmonisation\analyst\Tracy\rmonize\data_dictionary\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D8198F9-455C-4727-8D3B-F3AD2B908638}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED3FB69B-33C8-4E9B-BA27-98AD5D1D7A71}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Variables" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="324" uniqueCount="145">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="324" uniqueCount="147">
   <si>
     <t>index</t>
   </si>
@@ -95,9 +95,6 @@
     <t>packyear_tabacco</t>
   </si>
   <si>
-    <t>Packyears (cigarettes/cigars/pipes)</t>
-  </si>
-  <si>
     <t>Currently nr. smoked cigarettes/day</t>
   </si>
   <si>
@@ -110,42 +107,27 @@
     <t>vit_min</t>
   </si>
   <si>
-    <t>Vitamine, Mineralstoffe (J/N)</t>
-  </si>
-  <si>
     <t>fr_hrt1</t>
   </si>
   <si>
-    <t>No. biol. children</t>
-  </si>
-  <si>
     <t>Number of biological children</t>
   </si>
   <si>
     <t>diabetes2</t>
   </si>
   <si>
-    <t>Diabetes (interview or antidiabetic med)</t>
-  </si>
-  <si>
     <t>hyp_i</t>
   </si>
   <si>
     <t>htn_kora</t>
   </si>
   <si>
-    <t>Physician diagnosed hypertension (self reported)</t>
-  </si>
-  <si>
     <t>Hypertension:&gt;=140/90 or drugs(ATC) if known htn</t>
   </si>
   <si>
     <t>cancer</t>
   </si>
   <si>
-    <t>Cancer ever (interview)</t>
-  </si>
-  <si>
     <t>cvd</t>
   </si>
   <si>
@@ -155,39 +137,21 @@
     <t>fam_stroke</t>
   </si>
   <si>
-    <t>Family history of stroke (parents or sibling)</t>
-  </si>
-  <si>
     <t>fam_diab</t>
   </si>
   <si>
     <t>fam_cancer</t>
   </si>
   <si>
-    <t>Family history of dm (parents or sibling)</t>
-  </si>
-  <si>
-    <t>Family history of cancer (parents or sibling)</t>
-  </si>
-  <si>
     <t xml:space="preserve">  f2_mi_i_inc</t>
   </si>
   <si>
-    <t>Myocard.infarct since Carla_1 - Carla_2 (interview)</t>
-  </si>
-  <si>
     <t xml:space="preserve">f2_stoke_i_inc; </t>
   </si>
   <si>
-    <t>Stroke since Carla_1 - Carla_2 (interview)</t>
-  </si>
-  <si>
     <t>f1_stroke_first_year_inc</t>
   </si>
   <si>
-    <t>Year of 1st Stroke since Carla_0 - Carla_1 (interview)</t>
-  </si>
-  <si>
     <t>f1_chf_total_inz</t>
   </si>
   <si>
@@ -203,27 +167,15 @@
     <t>f2_cancer1_inc</t>
   </si>
   <si>
-    <t>Ist bei Ihnen seit Carla_1 eine Krebserkrankung neu aufgetreten? - Carla_2</t>
-  </si>
-  <si>
     <t>f2_cancer1_typ</t>
   </si>
   <si>
-    <t>Welche Krebserkrankung war das (I)? - Carla_2</t>
-  </si>
-  <si>
     <t>f2_cancer1_date</t>
   </si>
   <si>
-    <t>Wann ist diese Krebserkrankung zum ersten Mal diagnostiziert worden [Monat/Jahr] (I) - Carla_2</t>
-  </si>
-  <si>
     <t>vit_stat</t>
   </si>
   <si>
-    <t>Vital status (1=dead/0=alive))</t>
-  </si>
-  <si>
     <t>tod_dat</t>
   </si>
   <si>
@@ -242,15 +194,6 @@
     <t xml:space="preserve">elementary School </t>
   </si>
   <si>
-    <t xml:space="preserve"> secondary School (Realschule in FRG)</t>
-  </si>
-  <si>
-    <t>polytechn.secondary school (POS in GDR)</t>
-  </si>
-  <si>
-    <t>qualif. F.university of applied sciences (Fachholschulreife)</t>
-  </si>
-  <si>
     <t>A-levels/university entrance qualif.(Abitur)</t>
   </si>
   <si>
@@ -278,9 +221,6 @@
     <t>in education/re-education</t>
   </si>
   <si>
-    <t xml:space="preserve">student, </t>
-  </si>
-  <si>
     <t>maternity or other leave</t>
   </si>
   <si>
@@ -329,12 +269,6 @@
     <t>No</t>
   </si>
   <si>
-    <t>No / don't know</t>
-  </si>
-  <si>
-    <t>8= I don't know</t>
-  </si>
-  <si>
     <t>educ3</t>
   </si>
   <si>
@@ -353,30 +287,12 @@
     <t>Highest professional qualification</t>
   </si>
   <si>
-    <t>School + occupational education</t>
-  </si>
-  <si>
-    <t>School + occupational education (3 groups)</t>
-  </si>
-  <si>
     <t>no vocational education</t>
   </si>
   <si>
     <t>training period</t>
   </si>
   <si>
-    <t>apprenticeship (Lehre)</t>
-  </si>
-  <si>
-    <t>vocational school (Berufsschule)</t>
-  </si>
-  <si>
-    <t>technical school (Fachschule)</t>
-  </si>
-  <si>
-    <t>university of applied sciences (Fachhochschule)</t>
-  </si>
-  <si>
     <t>university</t>
   </si>
   <si>
@@ -410,21 +326,9 @@
     <t>any sch.+appl.uni,uni</t>
   </si>
   <si>
-    <t>Educ1,2,3 (max sec.school+no occup.training)</t>
-  </si>
-  <si>
-    <t>Educ4,5 (sec.school+vocational school)</t>
-  </si>
-  <si>
-    <t>Educ6,7 (A-level+any/any school+univ.)</t>
-  </si>
-  <si>
     <t>f2_mi_year</t>
   </si>
   <si>
-    <t>Year of myocard.infarction since Carla_1 - Carla_2 (interview)</t>
-  </si>
-  <si>
     <t>Brustkrebs</t>
   </si>
   <si>
@@ -456,6 +360,108 @@
   </si>
   <si>
     <t>occup_edu_2</t>
+  </si>
+  <si>
+    <t>I don't know</t>
+  </si>
+  <si>
+    <t>No/don't know</t>
+  </si>
+  <si>
+    <t>don't know</t>
+  </si>
+  <si>
+    <t>student</t>
+  </si>
+  <si>
+    <t>apprenticeship(Lehre)</t>
+  </si>
+  <si>
+    <t>polytechn.secondary school(POS in GDR)</t>
+  </si>
+  <si>
+    <t>qualif. F.university of applied sciences(Fachholschulreife)</t>
+  </si>
+  <si>
+    <t>vocational school(Berufsschule)</t>
+  </si>
+  <si>
+    <t>technical school(Fachschule)</t>
+  </si>
+  <si>
+    <t>university of applied sciences(Fachhochschule)</t>
+  </si>
+  <si>
+    <t>Educ1,2,3(max sec.school+no occup.training)</t>
+  </si>
+  <si>
+    <t>Educ4,5(sec.school+vocational school)</t>
+  </si>
+  <si>
+    <t>Educ6,7(A-level+any/any school+univ.)</t>
+  </si>
+  <si>
+    <t>Packyears(cigarettes/cigars/pipes)</t>
+  </si>
+  <si>
+    <t>Vitamine, Mineralstoffe(J/N)</t>
+  </si>
+  <si>
+    <t>Diabetes(interview or antidiabetic med)</t>
+  </si>
+  <si>
+    <t>Physician diagnosed hypertension(self reported)</t>
+  </si>
+  <si>
+    <t>Cancer ever(interview)</t>
+  </si>
+  <si>
+    <t>Family history of stroke(parents or sibling)</t>
+  </si>
+  <si>
+    <t>Family history of dm(parents or sibling)</t>
+  </si>
+  <si>
+    <t>Family history of cancer(parents or sibling)</t>
+  </si>
+  <si>
+    <t>Vital status(1=dead/0=alive))</t>
+  </si>
+  <si>
+    <t>Welche Krebserkrankung war das(I)?-Carla_2</t>
+  </si>
+  <si>
+    <t>children</t>
+  </si>
+  <si>
+    <t>datetime</t>
+  </si>
+  <si>
+    <t>School+occupational education</t>
+  </si>
+  <si>
+    <t>School+occupational education(3 groups)</t>
+  </si>
+  <si>
+    <t>Myocard.infarct since Carla_1-Carla_2(interview)</t>
+  </si>
+  <si>
+    <t>Year of myocard.infarction since Carla_1-Carla_2(interview)</t>
+  </si>
+  <si>
+    <t>Stroke since Carla_1-Carla_2(interview)</t>
+  </si>
+  <si>
+    <t>Year of 1st Stroke since Carla_0-Carla_1(interview)</t>
+  </si>
+  <si>
+    <t>Ist bei Ihnen seit Carla_1 eine Krebserkrankung neu aufgetreten?-Carla_2</t>
+  </si>
+  <si>
+    <t>Wann ist diese Krebserkrankung zum ersten Mal diagnostiziert worden[Monat/Jahr](I)-Carla_2</t>
+  </si>
+  <si>
+    <t>secondary School(Realschule in FRG)</t>
   </si>
 </sst>
 </file>
@@ -947,8 +953,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:P40"/>
   <sheetViews>
-    <sheetView topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="B39" sqref="B39"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="E21" sqref="E21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1017,10 +1023,10 @@
     </row>
     <row r="6" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B6" s="21" t="s">
-        <v>106</v>
+        <v>84</v>
       </c>
       <c r="C6" s="25" t="s">
-        <v>107</v>
+        <v>85</v>
       </c>
       <c r="D6" s="9" t="s">
         <v>7</v>
@@ -1028,10 +1034,10 @@
     </row>
     <row r="7" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B7" s="21" t="s">
-        <v>120</v>
+        <v>92</v>
       </c>
       <c r="C7" s="25" t="s">
-        <v>108</v>
+        <v>86</v>
       </c>
       <c r="D7" s="9" t="s">
         <v>7</v>
@@ -1039,10 +1045,10 @@
     </row>
     <row r="8" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B8" s="21" t="s">
-        <v>121</v>
+        <v>93</v>
       </c>
       <c r="C8" s="25" t="s">
-        <v>109</v>
+        <v>87</v>
       </c>
       <c r="D8" s="9" t="s">
         <v>7</v>
@@ -1050,10 +1056,10 @@
     </row>
     <row r="9" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B9" s="21" t="s">
-        <v>105</v>
+        <v>83</v>
       </c>
       <c r="C9" s="25" t="s">
-        <v>110</v>
+        <v>138</v>
       </c>
       <c r="D9" s="9" t="s">
         <v>7</v>
@@ -1061,10 +1067,10 @@
     </row>
     <row r="10" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B10" s="21" t="s">
-        <v>104</v>
+        <v>82</v>
       </c>
       <c r="C10" s="21" t="s">
-        <v>111</v>
+        <v>139</v>
       </c>
       <c r="D10" s="9" t="s">
         <v>7</v>
@@ -1125,12 +1131,12 @@
         <v>7</v>
       </c>
     </row>
-    <row r="16" spans="1:4" s="7" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B16" s="5" t="s">
         <v>23</v>
       </c>
       <c r="C16" s="5" t="s">
-        <v>24</v>
+        <v>126</v>
       </c>
       <c r="D16" s="9" t="s">
         <v>20</v>
@@ -1141,7 +1147,7 @@
         <v>22</v>
       </c>
       <c r="C17" s="5" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D17" s="9" t="s">
         <v>20</v>
@@ -1149,10 +1155,10 @@
     </row>
     <row r="18" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B18" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="C18" s="5" t="s">
         <v>26</v>
-      </c>
-      <c r="C18" s="5" t="s">
-        <v>27</v>
       </c>
       <c r="D18" s="9" t="s">
         <v>20</v>
@@ -1160,10 +1166,10 @@
     </row>
     <row r="19" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B19" s="5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C19" s="5" t="s">
-        <v>29</v>
+        <v>127</v>
       </c>
       <c r="D19" s="9" t="s">
         <v>7</v>
@@ -1171,43 +1177,43 @@
     </row>
     <row r="20" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B20" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="C20" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="D20" s="9" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="21" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B21" s="22" t="s">
+        <v>136</v>
+      </c>
+      <c r="C21" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="D21" s="9" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="22" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B22" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="C20" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="D20" s="9" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="21" spans="2:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="B21" s="5" t="s">
+      <c r="C22" s="5" t="s">
+        <v>128</v>
+      </c>
+      <c r="D22" s="9" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="23" spans="2:4" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B23" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="C21" s="5" t="s">
-        <v>32</v>
-      </c>
-      <c r="D21" s="9" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="22" spans="2:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="B22" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="C22" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="D22" s="9" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="23" spans="2:4" s="7" customFormat="1" ht="45" x14ac:dyDescent="0.25">
-      <c r="B23" s="6" t="s">
-        <v>35</v>
-      </c>
       <c r="C23" s="6" t="s">
-        <v>37</v>
+        <v>129</v>
       </c>
       <c r="D23" s="7" t="s">
         <v>7</v>
@@ -1215,10 +1221,10 @@
     </row>
     <row r="24" spans="2:4" s="7" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="B24" s="6" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="C24" s="6" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="D24" s="7" t="s">
         <v>7</v>
@@ -1226,10 +1232,10 @@
     </row>
     <row r="25" spans="2:4" s="7" customFormat="1" ht="60" x14ac:dyDescent="0.25">
       <c r="B25" s="5" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
       <c r="C25" s="5" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
       <c r="D25" s="9" t="s">
         <v>7</v>
@@ -1237,32 +1243,32 @@
     </row>
     <row r="26" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B26" s="5" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="C26" s="5" t="s">
-        <v>40</v>
+        <v>130</v>
       </c>
       <c r="D26" s="9" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="27" spans="2:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B27" s="5" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
       <c r="C27" s="5" t="s">
-        <v>44</v>
+        <v>131</v>
       </c>
       <c r="D27" s="9" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="28" spans="2:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B28" s="5" t="s">
-        <v>45</v>
+        <v>38</v>
       </c>
       <c r="C28" s="5" t="s">
-        <v>47</v>
+        <v>132</v>
       </c>
       <c r="D28" s="9" t="s">
         <v>7</v>
@@ -1270,10 +1276,10 @@
     </row>
     <row r="29" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B29" s="5" t="s">
-        <v>46</v>
+        <v>39</v>
       </c>
       <c r="C29" s="5" t="s">
-        <v>48</v>
+        <v>133</v>
       </c>
       <c r="D29" s="9" t="s">
         <v>7</v>
@@ -1281,10 +1287,10 @@
     </row>
     <row r="30" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B30" s="10" t="s">
-        <v>49</v>
+        <v>40</v>
       </c>
       <c r="C30" s="8" t="s">
-        <v>50</v>
+        <v>140</v>
       </c>
       <c r="D30" s="9" t="s">
         <v>7</v>
@@ -1292,21 +1298,21 @@
     </row>
     <row r="31" spans="2:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B31" s="11" t="s">
-        <v>132</v>
+        <v>101</v>
       </c>
       <c r="C31" s="11" t="s">
-        <v>133</v>
+        <v>141</v>
       </c>
       <c r="D31" s="2" t="s">
-        <v>20</v>
+        <v>137</v>
       </c>
     </row>
     <row r="32" spans="2:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B32" s="4" t="s">
-        <v>51</v>
+        <v>41</v>
       </c>
       <c r="C32" s="11" t="s">
-        <v>52</v>
+        <v>142</v>
       </c>
       <c r="D32" s="2" t="s">
         <v>7</v>
@@ -1314,21 +1320,21 @@
     </row>
     <row r="33" spans="2:16" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B33" s="11" t="s">
-        <v>53</v>
+        <v>42</v>
       </c>
       <c r="C33" s="11" t="s">
-        <v>54</v>
+        <v>143</v>
       </c>
       <c r="D33" s="2" t="s">
-        <v>20</v>
+        <v>137</v>
       </c>
     </row>
     <row r="34" spans="2:16" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B34" s="21" t="s">
-        <v>55</v>
+        <v>43</v>
       </c>
       <c r="C34" s="21" t="s">
-        <v>56</v>
+        <v>44</v>
       </c>
       <c r="D34" s="22" t="s">
         <v>7</v>
@@ -1348,13 +1354,13 @@
     </row>
     <row r="35" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B35" s="12" t="s">
-        <v>57</v>
+        <v>45</v>
       </c>
       <c r="C35" s="12" t="s">
-        <v>58</v>
+        <v>46</v>
       </c>
       <c r="D35" s="8" t="s">
-        <v>20</v>
+        <v>137</v>
       </c>
       <c r="E35" s="8"/>
       <c r="F35" s="8"/>
@@ -1371,43 +1377,43 @@
     </row>
     <row r="36" spans="2:16" ht="30" x14ac:dyDescent="0.25">
       <c r="B36" s="12" t="s">
-        <v>59</v>
+        <v>47</v>
       </c>
       <c r="C36" s="12" t="s">
-        <v>60</v>
+        <v>144</v>
       </c>
       <c r="D36" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="37" spans="2:16" ht="45" x14ac:dyDescent="0.25">
+    <row r="37" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B37" s="12" t="s">
-        <v>61</v>
+        <v>48</v>
       </c>
       <c r="C37" s="12" t="s">
-        <v>62</v>
+        <v>135</v>
       </c>
       <c r="D37" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="38" spans="2:16" ht="90" x14ac:dyDescent="0.25">
+    <row r="38" spans="2:16" ht="30" x14ac:dyDescent="0.25">
       <c r="B38" s="12" t="s">
-        <v>63</v>
+        <v>49</v>
       </c>
       <c r="C38" s="12" t="s">
-        <v>64</v>
+        <v>145</v>
       </c>
       <c r="D38" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="39" spans="2:16" ht="30" x14ac:dyDescent="0.25">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="39" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B39" s="12" t="s">
-        <v>65</v>
+        <v>50</v>
       </c>
       <c r="C39" s="12" t="s">
-        <v>66</v>
+        <v>134</v>
       </c>
       <c r="D39" t="s">
         <v>7</v>
@@ -1415,13 +1421,13 @@
     </row>
     <row r="40" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B40" s="12" t="s">
-        <v>67</v>
+        <v>51</v>
       </c>
       <c r="C40" s="12" t="s">
-        <v>68</v>
+        <v>52</v>
       </c>
       <c r="D40" t="s">
-        <v>20</v>
+        <v>137</v>
       </c>
     </row>
   </sheetData>
@@ -1434,8 +1440,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:C102"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="D22" sqref="D22:D23"/>
+    <sheetView topLeftCell="A73" workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1464,7 +1470,7 @@
         <v>1</v>
       </c>
       <c r="C2" t="s">
-        <v>69</v>
+        <v>53</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
@@ -1475,7 +1481,7 @@
         <v>2</v>
       </c>
       <c r="C3" t="s">
-        <v>70</v>
+        <v>54</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
@@ -1486,7 +1492,7 @@
         <v>1</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>71</v>
+        <v>55</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
@@ -1497,7 +1503,7 @@
         <v>2</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>72</v>
+        <v>56</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="30" x14ac:dyDescent="0.25">
@@ -1508,7 +1514,7 @@
         <v>3</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>73</v>
+        <v>146</v>
       </c>
     </row>
     <row r="7" spans="1:3" ht="30" x14ac:dyDescent="0.25">
@@ -1519,10 +1525,10 @@
         <v>4</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A8" s="14" t="s">
         <v>10</v>
       </c>
@@ -1530,7 +1536,7 @@
         <v>5</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>75</v>
+        <v>119</v>
       </c>
     </row>
     <row r="9" spans="1:3" ht="45" x14ac:dyDescent="0.25">
@@ -1541,7 +1547,7 @@
         <v>6</v>
       </c>
       <c r="C9" s="5" t="s">
-        <v>76</v>
+        <v>57</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
@@ -1552,381 +1558,381 @@
         <v>7</v>
       </c>
       <c r="C10" s="14" t="s">
-        <v>77</v>
+        <v>58</v>
       </c>
     </row>
     <row r="11" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A11" s="21" t="s">
-        <v>106</v>
+        <v>84</v>
       </c>
       <c r="B11">
         <v>1</v>
       </c>
       <c r="C11" s="22" t="s">
-        <v>112</v>
+        <v>88</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" s="21" t="s">
-        <v>106</v>
+        <v>84</v>
       </c>
       <c r="B12">
         <v>2</v>
       </c>
       <c r="C12" s="22" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" s="21" t="s">
-        <v>106</v>
+        <v>84</v>
       </c>
       <c r="B13">
         <v>3</v>
       </c>
       <c r="C13" s="22" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" s="21" t="s">
-        <v>106</v>
+        <v>84</v>
       </c>
       <c r="B14">
         <v>4</v>
       </c>
       <c r="C14" s="22" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" s="21" t="s">
-        <v>106</v>
+        <v>84</v>
       </c>
       <c r="B15">
         <v>5</v>
       </c>
       <c r="C15" s="22" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A16" s="21" t="s">
-        <v>106</v>
+        <v>84</v>
       </c>
       <c r="B16">
         <v>6</v>
       </c>
       <c r="C16" s="22" t="s">
-        <v>117</v>
+        <v>122</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" s="21" t="s">
-        <v>106</v>
+        <v>84</v>
       </c>
       <c r="B17">
         <v>7</v>
       </c>
       <c r="C17" s="22" t="s">
-        <v>118</v>
+        <v>90</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" s="21" t="s">
-        <v>106</v>
+        <v>84</v>
       </c>
       <c r="B18">
         <v>8</v>
       </c>
       <c r="C18" s="22" t="s">
-        <v>119</v>
+        <v>91</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" s="21" t="s">
-        <v>144</v>
+        <v>112</v>
       </c>
       <c r="B19">
         <v>1</v>
       </c>
       <c r="C19" s="22" t="s">
-        <v>112</v>
+        <v>88</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" s="21" t="s">
-        <v>120</v>
+        <v>92</v>
       </c>
       <c r="B20">
         <v>2</v>
       </c>
       <c r="C20" s="22" t="s">
-        <v>113</v>
+        <v>89</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" s="21" t="s">
-        <v>144</v>
+        <v>112</v>
       </c>
       <c r="B21">
         <v>3</v>
       </c>
       <c r="C21" s="22" t="s">
-        <v>114</v>
+        <v>117</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" s="21" t="s">
-        <v>143</v>
+        <v>111</v>
       </c>
       <c r="B22">
         <v>4</v>
       </c>
       <c r="C22" s="22" t="s">
-        <v>115</v>
+        <v>120</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" s="21" t="s">
-        <v>143</v>
+        <v>111</v>
       </c>
       <c r="B23">
         <v>5</v>
       </c>
       <c r="C23" s="22" t="s">
-        <v>116</v>
+        <v>121</v>
       </c>
     </row>
     <row r="24" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A24" s="21" t="s">
-        <v>120</v>
+        <v>92</v>
       </c>
       <c r="B24">
         <v>6</v>
       </c>
       <c r="C24" s="22" t="s">
-        <v>117</v>
+        <v>122</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" s="21" t="s">
-        <v>120</v>
+        <v>92</v>
       </c>
       <c r="B25">
         <v>7</v>
       </c>
       <c r="C25" s="22" t="s">
-        <v>118</v>
+        <v>90</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" s="21" t="s">
-        <v>120</v>
+        <v>92</v>
       </c>
       <c r="B26">
         <v>8</v>
       </c>
       <c r="C26" s="22" t="s">
-        <v>119</v>
+        <v>91</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" s="21" t="s">
-        <v>121</v>
+        <v>93</v>
       </c>
       <c r="B27">
         <v>1</v>
       </c>
       <c r="C27" s="22" t="s">
-        <v>112</v>
+        <v>88</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" s="21" t="s">
-        <v>121</v>
+        <v>93</v>
       </c>
       <c r="B28">
         <v>2</v>
       </c>
       <c r="C28" s="22" t="s">
-        <v>113</v>
+        <v>89</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" s="21" t="s">
-        <v>121</v>
+        <v>93</v>
       </c>
       <c r="B29">
         <v>3</v>
       </c>
       <c r="C29" s="22" t="s">
-        <v>114</v>
+        <v>117</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" s="21" t="s">
-        <v>121</v>
+        <v>93</v>
       </c>
       <c r="B30">
         <v>4</v>
       </c>
       <c r="C30" s="22" t="s">
-        <v>115</v>
+        <v>120</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" s="21" t="s">
-        <v>121</v>
+        <v>93</v>
       </c>
       <c r="B31">
         <v>5</v>
       </c>
       <c r="C31" s="22" t="s">
-        <v>116</v>
+        <v>121</v>
       </c>
     </row>
     <row r="32" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A32" s="21" t="s">
-        <v>121</v>
+        <v>93</v>
       </c>
       <c r="B32">
         <v>6</v>
       </c>
       <c r="C32" s="22" t="s">
-        <v>117</v>
+        <v>122</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" s="21" t="s">
-        <v>121</v>
+        <v>93</v>
       </c>
       <c r="B33">
         <v>7</v>
       </c>
       <c r="C33" s="22" t="s">
-        <v>118</v>
+        <v>90</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34" s="21" t="s">
-        <v>121</v>
+        <v>93</v>
       </c>
       <c r="B34">
         <v>8</v>
       </c>
       <c r="C34" s="22" t="s">
-        <v>119</v>
+        <v>91</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35" s="21" t="s">
-        <v>105</v>
+        <v>83</v>
       </c>
       <c r="B35">
         <v>1</v>
       </c>
       <c r="C35" s="22" t="s">
-        <v>122</v>
+        <v>94</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A36" s="21" t="s">
-        <v>105</v>
+        <v>83</v>
       </c>
       <c r="B36">
         <v>2</v>
       </c>
       <c r="C36" s="22" t="s">
-        <v>123</v>
+        <v>95</v>
       </c>
     </row>
     <row r="37" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A37" s="21" t="s">
-        <v>105</v>
+        <v>83</v>
       </c>
       <c r="B37">
         <v>3</v>
       </c>
       <c r="C37" s="22" t="s">
-        <v>124</v>
+        <v>96</v>
       </c>
     </row>
     <row r="38" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A38" s="21" t="s">
-        <v>105</v>
+        <v>83</v>
       </c>
       <c r="B38">
         <v>4</v>
       </c>
       <c r="C38" s="22" t="s">
-        <v>125</v>
+        <v>97</v>
       </c>
     </row>
     <row r="39" spans="1:3" ht="45" x14ac:dyDescent="0.25">
       <c r="A39" s="21" t="s">
-        <v>105</v>
+        <v>83</v>
       </c>
       <c r="B39">
         <v>5</v>
       </c>
       <c r="C39" s="22" t="s">
-        <v>126</v>
+        <v>98</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A40" s="21" t="s">
-        <v>105</v>
+        <v>83</v>
       </c>
       <c r="B40">
         <v>6</v>
       </c>
       <c r="C40" s="22" t="s">
-        <v>127</v>
+        <v>99</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A41" s="21" t="s">
-        <v>105</v>
+        <v>83</v>
       </c>
       <c r="B41">
         <v>7</v>
       </c>
       <c r="C41" s="22" t="s">
-        <v>128</v>
+        <v>100</v>
       </c>
     </row>
     <row r="42" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A42" s="21" t="s">
-        <v>104</v>
+        <v>82</v>
       </c>
       <c r="B42">
         <v>1</v>
       </c>
       <c r="C42" s="22" t="s">
-        <v>129</v>
+        <v>123</v>
       </c>
     </row>
     <row r="43" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A43" s="21" t="s">
-        <v>104</v>
+        <v>82</v>
       </c>
       <c r="B43">
         <v>2</v>
       </c>
       <c r="C43" s="22" t="s">
-        <v>130</v>
+        <v>124</v>
       </c>
     </row>
     <row r="44" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A44" s="21" t="s">
-        <v>104</v>
+        <v>82</v>
       </c>
       <c r="B44">
         <v>3</v>
       </c>
       <c r="C44" s="22" t="s">
-        <v>131</v>
+        <v>125</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.25">
@@ -1937,7 +1943,7 @@
         <v>1</v>
       </c>
       <c r="C45" s="14" t="s">
-        <v>78</v>
+        <v>59</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.25">
@@ -1948,7 +1954,7 @@
         <v>2</v>
       </c>
       <c r="C46" s="14" t="s">
-        <v>79</v>
+        <v>60</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.25">
@@ -1959,7 +1965,7 @@
         <v>3</v>
       </c>
       <c r="C47" s="14" t="s">
-        <v>80</v>
+        <v>61</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.25">
@@ -1970,7 +1976,7 @@
         <v>1</v>
       </c>
       <c r="C48" s="24" t="s">
-        <v>81</v>
+        <v>62</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.25">
@@ -1981,7 +1987,7 @@
         <v>2</v>
       </c>
       <c r="C49" s="24" t="s">
-        <v>82</v>
+        <v>63</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.25">
@@ -1992,7 +1998,7 @@
         <v>3</v>
       </c>
       <c r="C50" s="24" t="s">
-        <v>83</v>
+        <v>64</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.25">
@@ -2003,7 +2009,7 @@
         <v>4</v>
       </c>
       <c r="C51" s="24" t="s">
-        <v>84</v>
+        <v>65</v>
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.25">
@@ -2014,7 +2020,7 @@
         <v>5</v>
       </c>
       <c r="C52" s="24" t="s">
-        <v>85</v>
+        <v>116</v>
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.25">
@@ -2025,7 +2031,7 @@
         <v>6</v>
       </c>
       <c r="C53" s="24" t="s">
-        <v>86</v>
+        <v>66</v>
       </c>
     </row>
     <row r="54" spans="1:3" ht="30" x14ac:dyDescent="0.25">
@@ -2036,7 +2042,7 @@
         <v>7</v>
       </c>
       <c r="C54" s="24" t="s">
-        <v>87</v>
+        <v>67</v>
       </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.25">
@@ -2047,7 +2053,7 @@
         <v>8</v>
       </c>
       <c r="C55" s="24" t="s">
-        <v>88</v>
+        <v>68</v>
       </c>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.25">
@@ -2058,7 +2064,7 @@
         <v>9</v>
       </c>
       <c r="C56" s="24" t="s">
-        <v>89</v>
+        <v>69</v>
       </c>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.25">
@@ -2069,7 +2075,7 @@
         <v>1</v>
       </c>
       <c r="C57" s="24" t="s">
-        <v>90</v>
+        <v>70</v>
       </c>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.25">
@@ -2080,7 +2086,7 @@
         <v>2</v>
       </c>
       <c r="C58" s="24" t="s">
-        <v>91</v>
+        <v>71</v>
       </c>
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.25">
@@ -2091,7 +2097,7 @@
         <v>3</v>
       </c>
       <c r="C59" s="24" t="s">
-        <v>92</v>
+        <v>72</v>
       </c>
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.25">
@@ -2102,458 +2108,458 @@
         <v>4</v>
       </c>
       <c r="C60" s="24" t="s">
-        <v>93</v>
+        <v>73</v>
       </c>
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A61" s="15" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B61">
         <v>1</v>
       </c>
       <c r="C61" s="14" t="s">
-        <v>94</v>
+        <v>74</v>
       </c>
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A62" s="15" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B62">
         <v>2</v>
       </c>
       <c r="C62" s="14" t="s">
-        <v>95</v>
+        <v>75</v>
       </c>
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A63" s="15" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B63">
         <v>9</v>
       </c>
       <c r="C63" s="14" t="s">
-        <v>96</v>
+        <v>76</v>
       </c>
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A64" s="14" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="B64">
         <v>0</v>
       </c>
       <c r="C64" s="14" t="s">
-        <v>95</v>
+        <v>75</v>
       </c>
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A65" s="14" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="B65">
         <v>1</v>
       </c>
       <c r="C65" s="14" t="s">
-        <v>94</v>
+        <v>74</v>
       </c>
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A66" s="15" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
       <c r="B66">
         <v>0</v>
       </c>
       <c r="C66" s="14" t="s">
-        <v>95</v>
+        <v>75</v>
       </c>
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A67" s="15" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
       <c r="B67">
         <v>1</v>
       </c>
       <c r="C67" s="14" t="s">
-        <v>97</v>
+        <v>77</v>
       </c>
     </row>
     <row r="68" spans="1:3" ht="45" x14ac:dyDescent="0.25">
       <c r="A68" s="15" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
       <c r="B68">
         <v>2</v>
       </c>
       <c r="C68" s="14" t="s">
-        <v>98</v>
+        <v>78</v>
       </c>
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A69" s="14" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="B69">
         <v>0</v>
       </c>
       <c r="C69" s="14" t="s">
-        <v>95</v>
+        <v>75</v>
       </c>
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A70" s="14" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="B70">
         <v>1</v>
       </c>
       <c r="C70" s="14" t="s">
-        <v>99</v>
+        <v>79</v>
       </c>
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A71" s="14" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
       <c r="B71">
         <v>1</v>
       </c>
       <c r="C71" s="14" t="s">
-        <v>100</v>
+        <v>80</v>
       </c>
     </row>
     <row r="72" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A72" s="14" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
       <c r="B72">
         <v>2</v>
       </c>
       <c r="C72" s="14" t="s">
-        <v>101</v>
+        <v>81</v>
       </c>
     </row>
     <row r="73" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A73" s="14" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
       <c r="B73">
         <v>3</v>
       </c>
       <c r="C73" s="14" t="s">
-        <v>102</v>
+        <v>114</v>
       </c>
     </row>
     <row r="74" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A74" s="14" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
       <c r="B74">
         <v>8</v>
       </c>
       <c r="C74" s="14" t="s">
-        <v>103</v>
+        <v>113</v>
       </c>
     </row>
     <row r="75" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A75" s="14" t="s">
-        <v>45</v>
+        <v>38</v>
       </c>
       <c r="B75">
         <v>1</v>
       </c>
       <c r="C75" s="14" t="s">
-        <v>100</v>
+        <v>80</v>
       </c>
     </row>
     <row r="76" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A76" s="14" t="s">
-        <v>45</v>
+        <v>38</v>
       </c>
       <c r="B76">
         <v>2</v>
       </c>
       <c r="C76" s="14" t="s">
-        <v>101</v>
+        <v>81</v>
       </c>
     </row>
     <row r="77" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A77" s="14" t="s">
-        <v>45</v>
+        <v>38</v>
       </c>
       <c r="B77">
         <v>3</v>
       </c>
       <c r="C77" s="14" t="s">
-        <v>102</v>
+        <v>114</v>
       </c>
     </row>
     <row r="78" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A78" s="14" t="s">
-        <v>45</v>
+        <v>38</v>
       </c>
       <c r="B78">
         <v>8</v>
       </c>
       <c r="C78" s="14" t="s">
-        <v>103</v>
+        <v>115</v>
       </c>
     </row>
     <row r="79" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A79" s="14" t="s">
-        <v>46</v>
+        <v>39</v>
       </c>
       <c r="B79">
         <v>1</v>
       </c>
       <c r="C79" s="14" t="s">
-        <v>100</v>
+        <v>80</v>
       </c>
     </row>
     <row r="80" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A80" s="14" t="s">
-        <v>46</v>
+        <v>39</v>
       </c>
       <c r="B80">
         <v>2</v>
       </c>
       <c r="C80" s="14" t="s">
-        <v>101</v>
+        <v>81</v>
       </c>
     </row>
     <row r="81" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A81" s="14" t="s">
-        <v>46</v>
+        <v>39</v>
       </c>
       <c r="B81">
         <v>3</v>
       </c>
       <c r="C81" s="14" t="s">
-        <v>102</v>
+        <v>114</v>
       </c>
     </row>
     <row r="82" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A82" s="14" t="s">
-        <v>46</v>
+        <v>39</v>
       </c>
       <c r="B82">
         <v>8</v>
       </c>
       <c r="C82" s="14" t="s">
-        <v>103</v>
+        <v>113</v>
       </c>
     </row>
     <row r="83" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A83" s="10" t="s">
-        <v>49</v>
+        <v>40</v>
       </c>
       <c r="B83" s="20">
         <v>1</v>
       </c>
       <c r="C83" s="20" t="s">
-        <v>94</v>
+        <v>74</v>
       </c>
     </row>
     <row r="84" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A84" s="10" t="s">
-        <v>49</v>
+        <v>40</v>
       </c>
       <c r="B84" s="20">
         <v>2</v>
       </c>
       <c r="C84" s="20" t="s">
-        <v>95</v>
+        <v>75</v>
       </c>
     </row>
     <row r="85" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A85" s="4" t="s">
-        <v>51</v>
+        <v>41</v>
       </c>
       <c r="B85">
         <v>1</v>
       </c>
       <c r="C85" s="17" t="s">
-        <v>94</v>
+        <v>74</v>
       </c>
     </row>
     <row r="86" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A86" s="4" t="s">
-        <v>51</v>
+        <v>41</v>
       </c>
       <c r="B86">
         <v>2</v>
       </c>
       <c r="C86" s="17" t="s">
-        <v>95</v>
+        <v>75</v>
       </c>
     </row>
     <row r="87" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
-        <v>55</v>
+        <v>43</v>
       </c>
       <c r="B87">
         <v>0</v>
       </c>
       <c r="C87" s="18" t="s">
-        <v>95</v>
+        <v>75</v>
       </c>
     </row>
     <row r="88" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
-        <v>55</v>
+        <v>43</v>
       </c>
       <c r="B88">
         <v>1</v>
       </c>
       <c r="C88" s="18" t="s">
-        <v>94</v>
+        <v>74</v>
       </c>
     </row>
     <row r="89" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A89" s="21" t="s">
-        <v>59</v>
+        <v>47</v>
       </c>
       <c r="B89" s="20">
         <v>1</v>
       </c>
       <c r="C89" s="20" t="s">
-        <v>94</v>
+        <v>74</v>
       </c>
     </row>
     <row r="90" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A90" s="21" t="s">
-        <v>59</v>
+        <v>47</v>
       </c>
       <c r="B90" s="20">
         <v>2</v>
       </c>
       <c r="C90" s="20" t="s">
-        <v>95</v>
+        <v>75</v>
       </c>
     </row>
     <row r="91" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A91" s="21" t="s">
-        <v>61</v>
+        <v>48</v>
       </c>
       <c r="B91" s="10">
         <v>1</v>
       </c>
       <c r="C91" s="10" t="s">
-        <v>134</v>
+        <v>102</v>
       </c>
     </row>
     <row r="92" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A92" s="21" t="s">
-        <v>61</v>
+        <v>48</v>
       </c>
       <c r="B92" s="10">
         <v>2</v>
       </c>
       <c r="C92" s="10" t="s">
-        <v>135</v>
+        <v>103</v>
       </c>
     </row>
     <row r="93" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A93" s="21" t="s">
-        <v>61</v>
+        <v>48</v>
       </c>
       <c r="B93" s="10">
         <v>3</v>
       </c>
       <c r="C93" s="10" t="s">
-        <v>136</v>
+        <v>104</v>
       </c>
     </row>
     <row r="94" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A94" s="21" t="s">
-        <v>61</v>
+        <v>48</v>
       </c>
       <c r="B94" s="10">
         <v>4</v>
       </c>
       <c r="C94" s="10" t="s">
-        <v>137</v>
+        <v>105</v>
       </c>
     </row>
     <row r="95" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A95" s="21" t="s">
-        <v>61</v>
+        <v>48</v>
       </c>
       <c r="B95" s="10">
         <v>5</v>
       </c>
       <c r="C95" s="10" t="s">
-        <v>138</v>
+        <v>106</v>
       </c>
     </row>
     <row r="96" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A96" s="21" t="s">
-        <v>61</v>
+        <v>48</v>
       </c>
       <c r="B96" s="10">
         <v>6</v>
       </c>
       <c r="C96" s="10" t="s">
-        <v>139</v>
+        <v>107</v>
       </c>
     </row>
     <row r="97" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A97" s="21" t="s">
-        <v>61</v>
+        <v>48</v>
       </c>
       <c r="B97" s="10">
         <v>7</v>
       </c>
       <c r="C97" s="10" t="s">
-        <v>140</v>
+        <v>108</v>
       </c>
     </row>
     <row r="98" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A98" s="21" t="s">
-        <v>61</v>
+        <v>48</v>
       </c>
       <c r="B98" s="10">
         <v>8</v>
       </c>
       <c r="C98" s="10" t="s">
-        <v>141</v>
+        <v>109</v>
       </c>
     </row>
     <row r="99" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A99" s="21" t="s">
-        <v>61</v>
+        <v>48</v>
       </c>
       <c r="B99" s="26">
         <v>9</v>
       </c>
       <c r="C99" s="10" t="s">
-        <v>142</v>
+        <v>110</v>
       </c>
     </row>
     <row r="100" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A100" s="21" t="s">
-        <v>65</v>
+        <v>50</v>
       </c>
       <c r="B100" s="26">
         <v>0</v>
       </c>
       <c r="C100" s="22" t="s">
-        <v>95</v>
+        <v>75</v>
       </c>
     </row>
     <row r="101" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A101" s="21" t="s">
-        <v>65</v>
+        <v>50</v>
       </c>
       <c r="B101" s="26">
         <v>1</v>
       </c>
       <c r="C101" s="22" t="s">
-        <v>94</v>
+        <v>74</v>
       </c>
     </row>
     <row r="102" spans="1:3" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
CARLA-3 Educ_level worked now :) It looks good now!
</commit_message>
<xml_diff>
--- a/analyst/Tracy/rmonize/data_dictionary/DD_CARLA_TRACY.xlsx
+++ b/analyst/Tracy/rmonize/data_dictionary/DD_CARLA_TRACY.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="K:\use-cases-harmonisation\use-cases-harmonisation\analyst\Tracy\rmonize\data_dictionary\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED3FB69B-33C8-4E9B-BA27-98AD5D1D7A71}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{11F51EEE-CA46-4541-9134-99B74F468573}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Variables" sheetId="1" r:id="rId1"/>
@@ -953,8 +953,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:P40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="E21" sqref="E21"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1440,8 +1440,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:C102"/>
   <sheetViews>
-    <sheetView topLeftCell="A73" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
CARLA-3 Employment:Repetition taking off. “marginal/irregular employed” mapped to other. Menopause:Extra info. Have been put back. valueType :all changed to date
</commit_message>
<xml_diff>
--- a/analyst/Tracy/rmonize/data_dictionary/DD_CARLA_TRACY.xlsx
+++ b/analyst/Tracy/rmonize/data_dictionary/DD_CARLA_TRACY.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="K:\use-cases-harmonisation\use-cases-harmonisation\analyst\Tracy\rmonize\data_dictionary\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E1030947-2113-465A-9FB5-B74D58152AA2}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{420990E5-7B66-4738-BA84-D50B2E805EE5}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Variables" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="279" uniqueCount="127">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="276" uniqueCount="128">
   <si>
     <t>index</t>
   </si>
@@ -314,9 +314,6 @@
     <t>children</t>
   </si>
   <si>
-    <t>datetime</t>
-  </si>
-  <si>
     <t>secondary School(Realschule in FRG)</t>
   </si>
   <si>
@@ -326,12 +323,6 @@
     <t>Currently nr. smoked pipes/day</t>
   </si>
   <si>
-    <t>tabacconr_day</t>
-  </si>
-  <si>
-    <t>Currently nr. smoked cigarettes,cigars,pipes /day</t>
-  </si>
-  <si>
     <t xml:space="preserve"> No</t>
   </si>
   <si>
@@ -402,6 +393,18 @@
   </si>
   <si>
     <t>Date of birth</t>
+  </si>
+  <si>
+    <t>yes (regular)</t>
+  </si>
+  <si>
+    <t>yes (irregular)</t>
+  </si>
+  <si>
+    <t>yes, one</t>
+  </si>
+  <si>
+    <t>yes, both(surgical ova.)</t>
   </si>
 </sst>
 </file>
@@ -882,10 +885,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:P39"/>
+  <dimension ref="A1:P38"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="D25" sqref="D25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -913,7 +916,7 @@
         <v>5</v>
       </c>
       <c r="C2" s="18" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="D2" s="18" t="s">
         <v>6</v>
@@ -1031,10 +1034,10 @@
     </row>
     <row r="13" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B13" s="16" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="C13" s="19" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="D13" s="6" t="s">
         <v>17</v>
@@ -1042,21 +1045,21 @@
     </row>
     <row r="14" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B14" s="19" t="s">
+        <v>98</v>
+      </c>
+      <c r="C14" s="19" t="s">
         <v>99</v>
-      </c>
-      <c r="C14" s="19" t="s">
-        <v>100</v>
       </c>
       <c r="D14" s="6" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="15" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B15" s="19" t="s">
-        <v>101</v>
-      </c>
-      <c r="C15" s="19" t="s">
-        <v>102</v>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B15" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="C15" s="3" t="s">
+        <v>23</v>
       </c>
       <c r="D15" s="6" t="s">
         <v>17</v>
@@ -1064,76 +1067,76 @@
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B16" s="3" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>23</v>
+        <v>88</v>
       </c>
       <c r="D16" s="6" t="s">
-        <v>17</v>
+        <v>6</v>
       </c>
     </row>
     <row r="17" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B17" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="C17" s="3" t="s">
-        <v>88</v>
+      <c r="B17" s="19" t="s">
+        <v>113</v>
+      </c>
+      <c r="C17" s="19" t="s">
+        <v>115</v>
       </c>
       <c r="D17" s="6" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="18" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B18" s="19" t="s">
+      <c r="B18" s="16" t="s">
+        <v>114</v>
+      </c>
+      <c r="C18" s="19" t="s">
         <v>116</v>
       </c>
-      <c r="C18" s="19" t="s">
-        <v>118</v>
-      </c>
       <c r="D18" s="6" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="19" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B19" s="16" t="s">
-        <v>117</v>
-      </c>
-      <c r="C19" s="19" t="s">
-        <v>119</v>
+      <c r="B19" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="C19" s="3" t="s">
+        <v>25</v>
       </c>
       <c r="D19" s="6" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="20" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B20" s="3" t="s">
-        <v>25</v>
+      <c r="B20" s="16" t="s">
+        <v>96</v>
       </c>
       <c r="C20" s="3" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="D20" s="6" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="21" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B21" s="16" t="s">
-        <v>96</v>
+      <c r="B21" s="3" t="s">
+        <v>27</v>
       </c>
       <c r="C21" s="3" t="s">
-        <v>26</v>
+        <v>89</v>
       </c>
       <c r="D21" s="6" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="22" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B22" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="C22" s="3" t="s">
-        <v>89</v>
+    <row r="22" spans="2:4" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B22" s="15" t="s">
+        <v>28</v>
+      </c>
+      <c r="C22" s="15" t="s">
+        <v>90</v>
       </c>
       <c r="D22" s="6" t="s">
         <v>6</v>
@@ -1141,43 +1144,43 @@
     </row>
     <row r="23" spans="2:4" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B23" s="15" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="C23" s="15" t="s">
-        <v>90</v>
+        <v>30</v>
       </c>
       <c r="D23" s="6" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="24" spans="2:4" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B24" s="15" t="s">
-        <v>29</v>
-      </c>
-      <c r="C24" s="15" t="s">
-        <v>30</v>
+      <c r="B24" s="6" t="s">
+        <v>119</v>
+      </c>
+      <c r="C24" s="18" t="s">
+        <v>120</v>
       </c>
       <c r="D24" s="6" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="25" spans="2:4" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B25" s="6" t="s">
-        <v>122</v>
-      </c>
-      <c r="C25" s="18" t="s">
-        <v>123</v>
+        <v>17</v>
+      </c>
+    </row>
+    <row r="25" spans="2:4" s="4" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="B25" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="C25" s="3" t="s">
+        <v>33</v>
       </c>
       <c r="D25" s="6" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="26" spans="2:4" s="4" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="26" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B26" s="3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C26" s="3" t="s">
-        <v>33</v>
+        <v>91</v>
       </c>
       <c r="D26" s="6" t="s">
         <v>6</v>
@@ -1185,10 +1188,10 @@
     </row>
     <row r="27" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B27" s="3" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="C27" s="3" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="D27" s="6" t="s">
         <v>6</v>
@@ -1196,10 +1199,10 @@
     </row>
     <row r="28" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B28" s="3" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="C28" s="3" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="D28" s="6" t="s">
         <v>6</v>
@@ -1207,21 +1210,21 @@
     </row>
     <row r="29" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B29" s="3" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="C29" s="3" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="D29" s="6" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="30" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B30" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="C30" s="3" t="s">
-        <v>94</v>
+      <c r="B30" s="6" t="s">
+        <v>102</v>
+      </c>
+      <c r="C30" s="6" t="s">
+        <v>104</v>
       </c>
       <c r="D30" s="6" t="s">
         <v>6</v>
@@ -1229,10 +1232,10 @@
     </row>
     <row r="31" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B31" s="6" t="s">
+        <v>103</v>
+      </c>
+      <c r="C31" s="6" t="s">
         <v>105</v>
-      </c>
-      <c r="C31" s="6" t="s">
-        <v>107</v>
       </c>
       <c r="D31" s="6" t="s">
         <v>6</v>
@@ -1242,7 +1245,7 @@
       <c r="B32" s="6" t="s">
         <v>106</v>
       </c>
-      <c r="C32" s="6" t="s">
+      <c r="C32" s="15" t="s">
         <v>108</v>
       </c>
       <c r="D32" s="6" t="s">
@@ -1251,103 +1254,92 @@
     </row>
     <row r="33" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B33" s="6" t="s">
+        <v>107</v>
+      </c>
+      <c r="C33" s="15" t="s">
         <v>109</v>
       </c>
-      <c r="C33" s="15" t="s">
+      <c r="D33" s="6" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="34" spans="2:16" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B34" s="15" t="s">
+        <v>37</v>
+      </c>
+      <c r="C34" s="15" t="s">
+        <v>38</v>
+      </c>
+      <c r="D34" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="E34" s="17"/>
+      <c r="F34" s="17"/>
+      <c r="G34" s="14"/>
+      <c r="H34" s="14"/>
+      <c r="I34" s="14"/>
+      <c r="J34" s="14"/>
+      <c r="K34" s="14"/>
+      <c r="L34" s="14"/>
+      <c r="M34" s="14"/>
+      <c r="N34" s="14"/>
+      <c r="O34" s="14"/>
+      <c r="P34" s="14"/>
+    </row>
+    <row r="35" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B35" s="15" t="s">
+        <v>112</v>
+      </c>
+      <c r="C35" s="7" t="s">
+        <v>122</v>
+      </c>
+      <c r="D35" s="5" t="s">
         <v>111</v>
       </c>
-      <c r="D33" s="6" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="34" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B34" s="6" t="s">
-        <v>110</v>
-      </c>
-      <c r="C34" s="15" t="s">
-        <v>112</v>
-      </c>
-      <c r="D34" s="6" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="35" spans="2:16" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B35" s="15" t="s">
-        <v>37</v>
-      </c>
-      <c r="C35" s="15" t="s">
-        <v>38</v>
-      </c>
-      <c r="D35" s="16" t="s">
-        <v>6</v>
-      </c>
-      <c r="E35" s="17"/>
-      <c r="F35" s="17"/>
-      <c r="G35" s="14"/>
-      <c r="H35" s="14"/>
-      <c r="I35" s="14"/>
-      <c r="J35" s="14"/>
-      <c r="K35" s="14"/>
-      <c r="L35" s="14"/>
-      <c r="M35" s="14"/>
-      <c r="N35" s="14"/>
-      <c r="O35" s="14"/>
-      <c r="P35" s="14"/>
+      <c r="E35" s="5"/>
+      <c r="F35" s="5"/>
+      <c r="G35" s="5"/>
+      <c r="H35" s="5"/>
+      <c r="I35" s="5"/>
+      <c r="J35" s="5"/>
+      <c r="K35" s="5"/>
+      <c r="L35" s="5"/>
+      <c r="M35" s="5"/>
+      <c r="N35" s="5"/>
+      <c r="O35" s="5"/>
+      <c r="P35" s="5"/>
     </row>
     <row r="36" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B36" s="15" t="s">
-        <v>115</v>
+      <c r="B36" s="7" t="s">
+        <v>39</v>
       </c>
       <c r="C36" s="7" t="s">
-        <v>125</v>
-      </c>
-      <c r="D36" s="5" t="s">
-        <v>114</v>
-      </c>
-      <c r="E36" s="5"/>
-      <c r="F36" s="5"/>
-      <c r="G36" s="5"/>
-      <c r="H36" s="5"/>
-      <c r="I36" s="5"/>
-      <c r="J36" s="5"/>
-      <c r="K36" s="5"/>
-      <c r="L36" s="5"/>
-      <c r="M36" s="5"/>
-      <c r="N36" s="5"/>
-      <c r="O36" s="5"/>
-      <c r="P36" s="5"/>
+        <v>95</v>
+      </c>
+      <c r="D36" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="37" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B37" s="7" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="C37" s="7" t="s">
-        <v>95</v>
+        <v>41</v>
       </c>
       <c r="D37" t="s">
-        <v>6</v>
+        <v>111</v>
       </c>
     </row>
     <row r="38" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B38" s="7" t="s">
-        <v>40</v>
-      </c>
-      <c r="C38" s="7" t="s">
-        <v>41</v>
+      <c r="B38" s="11" t="s">
+        <v>110</v>
+      </c>
+      <c r="C38" t="s">
+        <v>123</v>
       </c>
       <c r="D38" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="39" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B39" s="11" t="s">
-        <v>113</v>
-      </c>
-      <c r="C39" t="s">
-        <v>126</v>
-      </c>
-      <c r="D39" t="s">
-        <v>97</v>
+        <v>111</v>
       </c>
     </row>
   </sheetData>
@@ -1360,8 +1352,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:C81"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="C35" sqref="C35"/>
+    <sheetView topLeftCell="A61" workbookViewId="0">
+      <selection activeCell="C43" sqref="C43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1434,7 +1426,7 @@
         <v>3</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="7" spans="1:3" ht="30" x14ac:dyDescent="0.25">
@@ -1769,62 +1761,62 @@
     </row>
     <row r="37" spans="1:3" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A37" s="6" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="B37" s="24">
         <v>1</v>
       </c>
       <c r="C37" s="24" t="s">
-        <v>66</v>
+        <v>124</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A38" s="19" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="B38" s="24">
         <v>2</v>
       </c>
       <c r="C38" s="24" t="s">
-        <v>66</v>
+        <v>125</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A39" s="19" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="B39" s="24">
         <v>3</v>
       </c>
       <c r="C39" s="24" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A40" s="16" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="B40" s="24">
         <v>1</v>
       </c>
       <c r="C40" s="24" t="s">
-        <v>63</v>
+        <v>126</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A41" s="16" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="B41" s="24">
         <v>2</v>
       </c>
       <c r="C41" s="24" t="s">
-        <v>63</v>
+        <v>127</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A42" s="16" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="B42" s="6">
         <v>3</v>
@@ -1907,7 +1899,7 @@
         <v>2</v>
       </c>
       <c r="C49" s="15" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.25">
@@ -2121,7 +2113,7 @@
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A69" s="6" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="B69" s="22">
         <v>0</v>
@@ -2132,7 +2124,7 @@
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A70" s="6" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="B70" s="22">
         <v>1</v>
@@ -2143,7 +2135,7 @@
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A71" s="6" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="B71" s="22">
         <v>0</v>
@@ -2154,7 +2146,7 @@
     </row>
     <row r="72" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A72" s="6" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="B72" s="22">
         <v>1</v>
@@ -2165,7 +2157,7 @@
     </row>
     <row r="73" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A73" s="6" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="B73" s="16">
         <v>0</v>
@@ -2176,7 +2168,7 @@
     </row>
     <row r="74" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A74" s="6" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="B74" s="16">
         <v>1</v>
@@ -2187,7 +2179,7 @@
     </row>
     <row r="75" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A75" s="6" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="B75" s="16">
         <v>0</v>
@@ -2198,7 +2190,7 @@
     </row>
     <row r="76" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A76" s="6" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="B76" s="16">
         <v>1</v>

</xml_diff>

<commit_message>
Edu- correction with the codes as suggested Work- Corrected the codes as suggested.
</commit_message>
<xml_diff>
--- a/analyst/Tracy/rmonize/data_dictionary/DD_CARLA_TRACY.xlsx
+++ b/analyst/Tracy/rmonize/data_dictionary/DD_CARLA_TRACY.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="K:\use-cases-harmonisation\use-cases-harmonisation\analyst\Tracy\rmonize\data_dictionary\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{420990E5-7B66-4738-BA84-D50B2E805EE5}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1992EA0C-041F-48EC-AF19-0D6AFED14A91}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -158,9 +158,6 @@
     <t>no formal education</t>
   </si>
   <si>
-    <t xml:space="preserve">elementary School </t>
-  </si>
-  <si>
     <t>A-levels/university entrance qualif.(Abitur)</t>
   </si>
   <si>
@@ -405,6 +402,9 @@
   </si>
   <si>
     <t>yes, both(surgical ova.)</t>
+  </si>
+  <si>
+    <t>Hauptschule</t>
   </si>
 </sst>
 </file>
@@ -887,8 +887,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:P38"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="D25" sqref="D25"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L20" sqref="L20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -916,7 +916,7 @@
         <v>5</v>
       </c>
       <c r="C2" s="18" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="D2" s="18" t="s">
         <v>6</v>
@@ -957,10 +957,10 @@
     </row>
     <row r="6" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B6" s="15" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C6" s="19" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D6" s="6" t="s">
         <v>6</v>
@@ -1015,7 +1015,7 @@
         <v>20</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D11" s="6" t="s">
         <v>17</v>
@@ -1034,10 +1034,10 @@
     </row>
     <row r="13" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B13" s="16" t="s">
+        <v>116</v>
+      </c>
+      <c r="C13" s="19" t="s">
         <v>117</v>
-      </c>
-      <c r="C13" s="19" t="s">
-        <v>118</v>
       </c>
       <c r="D13" s="6" t="s">
         <v>17</v>
@@ -1045,10 +1045,10 @@
     </row>
     <row r="14" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B14" s="19" t="s">
+        <v>97</v>
+      </c>
+      <c r="C14" s="19" t="s">
         <v>98</v>
-      </c>
-      <c r="C14" s="19" t="s">
-        <v>99</v>
       </c>
       <c r="D14" s="6" t="s">
         <v>17</v>
@@ -1070,7 +1070,7 @@
         <v>24</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="D16" s="6" t="s">
         <v>6</v>
@@ -1078,10 +1078,10 @@
     </row>
     <row r="17" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B17" s="19" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="C17" s="19" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="D17" s="6" t="s">
         <v>6</v>
@@ -1089,10 +1089,10 @@
     </row>
     <row r="18" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B18" s="16" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C18" s="19" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="D18" s="6" t="s">
         <v>6</v>
@@ -1111,7 +1111,7 @@
     </row>
     <row r="20" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B20" s="16" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C20" s="3" t="s">
         <v>26</v>
@@ -1125,7 +1125,7 @@
         <v>27</v>
       </c>
       <c r="C21" s="3" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="D21" s="6" t="s">
         <v>6</v>
@@ -1136,7 +1136,7 @@
         <v>28</v>
       </c>
       <c r="C22" s="15" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="D22" s="6" t="s">
         <v>6</v>
@@ -1155,10 +1155,10 @@
     </row>
     <row r="24" spans="2:4" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B24" s="6" t="s">
+        <v>118</v>
+      </c>
+      <c r="C24" s="18" t="s">
         <v>119</v>
-      </c>
-      <c r="C24" s="18" t="s">
-        <v>120</v>
       </c>
       <c r="D24" s="6" t="s">
         <v>17</v>
@@ -1180,7 +1180,7 @@
         <v>31</v>
       </c>
       <c r="C26" s="3" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D26" s="6" t="s">
         <v>6</v>
@@ -1191,7 +1191,7 @@
         <v>34</v>
       </c>
       <c r="C27" s="3" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="D27" s="6" t="s">
         <v>6</v>
@@ -1202,7 +1202,7 @@
         <v>35</v>
       </c>
       <c r="C28" s="3" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D28" s="6" t="s">
         <v>6</v>
@@ -1213,7 +1213,7 @@
         <v>36</v>
       </c>
       <c r="C29" s="3" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="D29" s="6" t="s">
         <v>6</v>
@@ -1221,10 +1221,10 @@
     </row>
     <row r="30" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B30" s="6" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C30" s="6" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="D30" s="6" t="s">
         <v>6</v>
@@ -1232,10 +1232,10 @@
     </row>
     <row r="31" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B31" s="6" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C31" s="6" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="D31" s="6" t="s">
         <v>6</v>
@@ -1243,10 +1243,10 @@
     </row>
     <row r="32" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B32" s="6" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C32" s="15" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="D32" s="6" t="s">
         <v>6</v>
@@ -1254,10 +1254,10 @@
     </row>
     <row r="33" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B33" s="6" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C33" s="15" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="D33" s="6" t="s">
         <v>6</v>
@@ -1288,13 +1288,13 @@
     </row>
     <row r="35" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B35" s="15" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C35" s="7" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="D35" s="5" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="E35" s="5"/>
       <c r="F35" s="5"/>
@@ -1314,7 +1314,7 @@
         <v>39</v>
       </c>
       <c r="C36" s="7" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="D36" t="s">
         <v>6</v>
@@ -1328,18 +1328,18 @@
         <v>41</v>
       </c>
       <c r="D37" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="38" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B38" s="11" t="s">
+        <v>109</v>
+      </c>
+      <c r="C38" t="s">
+        <v>122</v>
+      </c>
+      <c r="D38" t="s">
         <v>110</v>
-      </c>
-      <c r="C38" t="s">
-        <v>123</v>
-      </c>
-      <c r="D38" t="s">
-        <v>111</v>
       </c>
     </row>
   </sheetData>
@@ -1352,8 +1352,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:C81"/>
   <sheetViews>
-    <sheetView topLeftCell="A61" workbookViewId="0">
-      <selection activeCell="C43" sqref="C43"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1414,8 +1414,8 @@
       <c r="B5">
         <v>2</v>
       </c>
-      <c r="C5" s="3" t="s">
-        <v>45</v>
+      <c r="C5" s="19" t="s">
+        <v>127</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="30" x14ac:dyDescent="0.25">
@@ -1426,7 +1426,7 @@
         <v>3</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="7" spans="1:3" ht="30" x14ac:dyDescent="0.25">
@@ -1437,7 +1437,7 @@
         <v>4</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="8" spans="1:3" ht="30" x14ac:dyDescent="0.25">
@@ -1448,7 +1448,7 @@
         <v>5</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="9" spans="1:3" ht="45" x14ac:dyDescent="0.25">
@@ -1459,7 +1459,7 @@
         <v>6</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
@@ -1470,95 +1470,95 @@
         <v>7</v>
       </c>
       <c r="C10" s="9" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" s="15" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B11">
         <v>1</v>
       </c>
       <c r="C11" s="16" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" s="15" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B12">
         <v>2</v>
       </c>
       <c r="C12" s="16" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" s="15" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B13">
         <v>3</v>
       </c>
       <c r="C13" s="16" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" s="15" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B14">
         <v>4</v>
       </c>
       <c r="C14" s="16" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" s="15" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B15">
         <v>5</v>
       </c>
       <c r="C15" s="16" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="16" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A16" s="15" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B16">
         <v>6</v>
       </c>
       <c r="C16" s="16" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" s="15" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B17">
         <v>7</v>
       </c>
       <c r="C17" s="16" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" s="15" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B18">
         <v>8</v>
       </c>
       <c r="C18" s="16" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
@@ -1569,7 +1569,7 @@
         <v>1</v>
       </c>
       <c r="C19" s="9" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
@@ -1580,7 +1580,7 @@
         <v>2</v>
       </c>
       <c r="C20" s="9" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
@@ -1591,7 +1591,7 @@
         <v>3</v>
       </c>
       <c r="C21" s="9" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
@@ -1602,7 +1602,7 @@
         <v>1</v>
       </c>
       <c r="C22" s="18" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
@@ -1613,7 +1613,7 @@
         <v>2</v>
       </c>
       <c r="C23" s="18" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
@@ -1624,7 +1624,7 @@
         <v>3</v>
       </c>
       <c r="C24" s="18" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
@@ -1635,7 +1635,7 @@
         <v>4</v>
       </c>
       <c r="C25" s="18" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
@@ -1646,7 +1646,7 @@
         <v>5</v>
       </c>
       <c r="C26" s="18" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
@@ -1657,7 +1657,7 @@
         <v>6</v>
       </c>
       <c r="C27" s="18" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="28" spans="1:3" ht="30" x14ac:dyDescent="0.25">
@@ -1668,7 +1668,7 @@
         <v>7</v>
       </c>
       <c r="C28" s="18" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
@@ -1679,7 +1679,7 @@
         <v>8</v>
       </c>
       <c r="C29" s="18" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
@@ -1690,7 +1690,7 @@
         <v>9</v>
       </c>
       <c r="C30" s="18" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
@@ -1701,7 +1701,7 @@
         <v>1</v>
       </c>
       <c r="C31" s="18" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
@@ -1712,7 +1712,7 @@
         <v>2</v>
       </c>
       <c r="C32" s="18" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
@@ -1723,7 +1723,7 @@
         <v>3</v>
       </c>
       <c r="C33" s="18" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
@@ -1734,7 +1734,7 @@
         <v>4</v>
       </c>
       <c r="C34" s="18" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
@@ -1745,7 +1745,7 @@
         <v>0</v>
       </c>
       <c r="C35" s="16" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.25">
@@ -1756,73 +1756,73 @@
         <v>1</v>
       </c>
       <c r="C36" s="16" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="37" spans="1:3" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A37" s="6" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B37" s="24">
         <v>1</v>
       </c>
       <c r="C37" s="24" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A38" s="19" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B38" s="24">
         <v>2</v>
       </c>
       <c r="C38" s="24" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A39" s="19" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B39" s="24">
         <v>3</v>
       </c>
       <c r="C39" s="24" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A40" s="16" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B40" s="24">
         <v>1</v>
       </c>
       <c r="C40" s="24" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A41" s="16" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B41" s="24">
         <v>2</v>
       </c>
       <c r="C41" s="24" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A42" s="16" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B42" s="6">
         <v>3</v>
       </c>
       <c r="C42" s="6" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.25">
@@ -1833,7 +1833,7 @@
         <v>1</v>
       </c>
       <c r="C43" s="9" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.25">
@@ -1844,7 +1844,7 @@
         <v>2</v>
       </c>
       <c r="C44" s="9" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.25">
@@ -1855,7 +1855,7 @@
         <v>9</v>
       </c>
       <c r="C45" s="9" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.25">
@@ -1866,7 +1866,7 @@
         <v>0</v>
       </c>
       <c r="C46" s="9" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.25">
@@ -1877,7 +1877,7 @@
         <v>1</v>
       </c>
       <c r="C47" s="9" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.25">
@@ -1888,7 +1888,7 @@
         <v>1</v>
       </c>
       <c r="C48" s="15" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.25">
@@ -1899,7 +1899,7 @@
         <v>2</v>
       </c>
       <c r="C49" s="15" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.25">
@@ -1910,7 +1910,7 @@
         <v>0</v>
       </c>
       <c r="C50" s="16" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.25">
@@ -1921,7 +1921,7 @@
         <v>1</v>
       </c>
       <c r="C51" s="16" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.25">
@@ -1932,7 +1932,7 @@
         <v>0</v>
       </c>
       <c r="C52" s="16" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.25">
@@ -1943,7 +1943,7 @@
         <v>1</v>
       </c>
       <c r="C53" s="9" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="54" spans="1:3" ht="45" x14ac:dyDescent="0.25">
@@ -1954,7 +1954,7 @@
         <v>2</v>
       </c>
       <c r="C54" s="9" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.25">
@@ -1965,7 +1965,7 @@
         <v>0</v>
       </c>
       <c r="C55" s="9" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.25">
@@ -1976,7 +1976,7 @@
         <v>1</v>
       </c>
       <c r="C56" s="9" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.25">
@@ -1987,7 +1987,7 @@
         <v>1</v>
       </c>
       <c r="C57" s="9" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.25">
@@ -1998,7 +1998,7 @@
         <v>2</v>
       </c>
       <c r="C58" s="9" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.25">
@@ -2009,7 +2009,7 @@
         <v>3</v>
       </c>
       <c r="C59" s="9" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.25">
@@ -2020,7 +2020,7 @@
         <v>8</v>
       </c>
       <c r="C60" s="9" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.25">
@@ -2031,7 +2031,7 @@
         <v>1</v>
       </c>
       <c r="C61" s="9" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.25">
@@ -2042,7 +2042,7 @@
         <v>2</v>
       </c>
       <c r="C62" s="9" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.25">
@@ -2053,7 +2053,7 @@
         <v>3</v>
       </c>
       <c r="C63" s="9" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.25">
@@ -2064,7 +2064,7 @@
         <v>8</v>
       </c>
       <c r="C64" s="9" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.25">
@@ -2075,7 +2075,7 @@
         <v>1</v>
       </c>
       <c r="C65" s="9" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.25">
@@ -2086,7 +2086,7 @@
         <v>2</v>
       </c>
       <c r="C66" s="9" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.25">
@@ -2097,7 +2097,7 @@
         <v>3</v>
       </c>
       <c r="C67" s="9" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.25">
@@ -2108,95 +2108,95 @@
         <v>8</v>
       </c>
       <c r="C68" s="9" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A69" s="6" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B69" s="22">
         <v>0</v>
       </c>
       <c r="C69" s="15" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A70" s="6" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B70" s="22">
         <v>1</v>
       </c>
       <c r="C70" s="15" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A71" s="6" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B71" s="22">
         <v>0</v>
       </c>
       <c r="C71" s="15" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="72" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A72" s="6" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B72" s="22">
         <v>1</v>
       </c>
       <c r="C72" s="15" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="73" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A73" s="6" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B73" s="16">
         <v>0</v>
       </c>
       <c r="C73" s="16" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="74" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A74" s="6" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B74" s="16">
         <v>1</v>
       </c>
       <c r="C74" s="16" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="75" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A75" s="6" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B75" s="16">
         <v>0</v>
       </c>
       <c r="C75" s="16" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="76" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A76" s="6" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B76" s="16">
         <v>1</v>
       </c>
       <c r="C76" s="16" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="77" spans="1:3" x14ac:dyDescent="0.25">
@@ -2207,7 +2207,7 @@
         <v>0</v>
       </c>
       <c r="C77" s="12" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="78" spans="1:3" x14ac:dyDescent="0.25">
@@ -2218,7 +2218,7 @@
         <v>1</v>
       </c>
       <c r="C78" s="12" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="79" spans="1:3" x14ac:dyDescent="0.25">
@@ -2229,7 +2229,7 @@
         <v>0</v>
       </c>
       <c r="C79" s="16" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="80" spans="1:3" x14ac:dyDescent="0.25">
@@ -2240,7 +2240,7 @@
         <v>1</v>
       </c>
       <c r="C80" s="16" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="81" spans="2:2" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
CARLA-3 1.	Added information how the medication variables (MED_STAT, MED_NSAID) were defined in the comment column: This is created according to ATC code C10AA and ATC code M01A and N02BA. 2.	AGE_HYP: We don’t have any information we can reference to, we think they have the information at their end. And they can do the calculations I will explain this in the email to Mr Kluttig. 3.	All dates changed to decimals
</commit_message>
<xml_diff>
--- a/analyst/Tracy/rmonize/data_dictionary/DD_CARLA_TRACY.xlsx
+++ b/analyst/Tracy/rmonize/data_dictionary/DD_CARLA_TRACY.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="K:\use-cases-harmonisation\use-cases-harmonisation\analyst\Tracy\rmonize\data_dictionary\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1992EA0C-041F-48EC-AF19-0D6AFED14A91}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{506F3012-0164-4A9F-B3B3-0E386DD33F67}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="276" uniqueCount="128">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="276" uniqueCount="127">
   <si>
     <t>index</t>
   </si>
@@ -351,9 +351,6 @@
   </si>
   <si>
     <t>gebdat</t>
-  </si>
-  <si>
-    <t>date</t>
   </si>
   <si>
     <t>f2_insuff_date</t>
@@ -888,7 +885,7 @@
   <dimension ref="A1:P38"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L20" sqref="L20"/>
+      <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1034,10 +1031,10 @@
     </row>
     <row r="13" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B13" s="16" t="s">
+        <v>115</v>
+      </c>
+      <c r="C13" s="19" t="s">
         <v>116</v>
-      </c>
-      <c r="C13" s="19" t="s">
-        <v>117</v>
       </c>
       <c r="D13" s="6" t="s">
         <v>17</v>
@@ -1078,10 +1075,10 @@
     </row>
     <row r="17" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B17" s="19" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C17" s="19" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="D17" s="6" t="s">
         <v>6</v>
@@ -1089,10 +1086,10 @@
     </row>
     <row r="18" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B18" s="16" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="C18" s="19" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="D18" s="6" t="s">
         <v>6</v>
@@ -1155,10 +1152,10 @@
     </row>
     <row r="24" spans="2:4" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B24" s="6" t="s">
+        <v>117</v>
+      </c>
+      <c r="C24" s="18" t="s">
         <v>118</v>
-      </c>
-      <c r="C24" s="18" t="s">
-        <v>119</v>
       </c>
       <c r="D24" s="6" t="s">
         <v>17</v>
@@ -1288,13 +1285,13 @@
     </row>
     <row r="35" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B35" s="15" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C35" s="7" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="D35" s="5" t="s">
-        <v>110</v>
+        <v>17</v>
       </c>
       <c r="E35" s="5"/>
       <c r="F35" s="5"/>
@@ -1328,7 +1325,7 @@
         <v>41</v>
       </c>
       <c r="D37" t="s">
-        <v>110</v>
+        <v>17</v>
       </c>
     </row>
     <row r="38" spans="2:16" x14ac:dyDescent="0.25">
@@ -1336,10 +1333,10 @@
         <v>109</v>
       </c>
       <c r="C38" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="D38" t="s">
-        <v>110</v>
+        <v>17</v>
       </c>
     </row>
   </sheetData>
@@ -1352,8 +1349,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:C81"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+    <sheetView topLeftCell="A64" workbookViewId="0">
+      <selection activeCell="C83" sqref="C83"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1415,7 +1412,7 @@
         <v>2</v>
       </c>
       <c r="C5" s="19" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="30" x14ac:dyDescent="0.25">
@@ -1761,62 +1758,62 @@
     </row>
     <row r="37" spans="1:3" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A37" s="6" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B37" s="24">
         <v>1</v>
       </c>
       <c r="C37" s="24" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A38" s="19" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B38" s="24">
         <v>2</v>
       </c>
       <c r="C38" s="24" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A39" s="19" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B39" s="24">
         <v>3</v>
       </c>
       <c r="C39" s="24" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A40" s="16" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B40" s="24">
         <v>1</v>
       </c>
       <c r="C40" s="24" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A41" s="16" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B41" s="24">
         <v>2</v>
       </c>
       <c r="C41" s="24" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A42" s="16" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B42" s="6">
         <v>3</v>
@@ -2159,7 +2156,7 @@
       <c r="A73" s="6" t="s">
         <v>105</v>
       </c>
-      <c r="B73" s="16">
+      <c r="B73" s="20">
         <v>0</v>
       </c>
       <c r="C73" s="16" t="s">
@@ -2170,7 +2167,7 @@
       <c r="A74" s="6" t="s">
         <v>105</v>
       </c>
-      <c r="B74" s="16">
+      <c r="B74" s="20">
         <v>1</v>
       </c>
       <c r="C74" s="16" t="s">
@@ -2181,7 +2178,7 @@
       <c r="A75" s="6" t="s">
         <v>106</v>
       </c>
-      <c r="B75" s="16">
+      <c r="B75" s="20">
         <v>0</v>
       </c>
       <c r="C75" s="16" t="s">
@@ -2192,7 +2189,7 @@
       <c r="A76" s="6" t="s">
         <v>106</v>
       </c>
-      <c r="B76" s="16">
+      <c r="B76" s="20">
         <v>1</v>
       </c>
       <c r="C76" s="16" t="s">

</xml_diff>

<commit_message>
CARLA-3 DD:tod_dat changed back to date DD:f2_insuff_date change back to date DD:gebdat changed back to date
</commit_message>
<xml_diff>
--- a/analyst/Tracy/rmonize/data_dictionary/DD_CARLA_TRACY.xlsx
+++ b/analyst/Tracy/rmonize/data_dictionary/DD_CARLA_TRACY.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="K:\use-cases-harmonisation\use-cases-harmonisation\analyst\Tracy\rmonize\data_dictionary\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{506F3012-0164-4A9F-B3B3-0E386DD33F67}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB3B4A16-0C84-44EE-908F-908C79D355FD}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="276" uniqueCount="127">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="276" uniqueCount="128">
   <si>
     <t>index</t>
   </si>
@@ -402,6 +402,9 @@
   </si>
   <si>
     <t>Hauptschule</t>
+  </si>
+  <si>
+    <t>date</t>
   </si>
 </sst>
 </file>
@@ -884,8 +887,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:P38"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="B40" sqref="B40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1291,7 +1294,7 @@
         <v>120</v>
       </c>
       <c r="D35" s="5" t="s">
-        <v>17</v>
+        <v>127</v>
       </c>
       <c r="E35" s="5"/>
       <c r="F35" s="5"/>
@@ -1325,7 +1328,7 @@
         <v>41</v>
       </c>
       <c r="D37" t="s">
-        <v>17</v>
+        <v>127</v>
       </c>
     </row>
     <row r="38" spans="2:16" x14ac:dyDescent="0.25">
@@ -1336,7 +1339,7 @@
         <v>121</v>
       </c>
       <c r="D38" t="s">
-        <v>17</v>
+        <v>127</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
CARLA-3 AGE_HYP:Changes madein Age at diagnosis of essential hypertension (years).
</commit_message>
<xml_diff>
--- a/analyst/Tracy/rmonize/data_dictionary/DD_CARLA_TRACY.xlsx
+++ b/analyst/Tracy/rmonize/data_dictionary/DD_CARLA_TRACY.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="K:\use-cases-harmonisation\use-cases-harmonisation\analyst\Tracy\rmonize\data_dictionary\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB3B4A16-0C84-44EE-908F-908C79D355FD}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D2ED5B10-F0A0-4A12-BBBA-E831CC763ACA}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="276" uniqueCount="128">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="282" uniqueCount="132">
   <si>
     <t>index</t>
   </si>
@@ -405,13 +405,49 @@
   </si>
   <si>
     <t>date</t>
+  </si>
+  <si>
+    <r>
+      <t>F1_untdat</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+  </si>
+  <si>
+    <t>baseline examination for follow-up 1</t>
+  </si>
+  <si>
+    <r>
+      <t>F2_untdat</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+  </si>
+  <si>
+    <t>baseline examination for follow-up 2</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -458,6 +494,13 @@
       <i/>
       <sz val="11"/>
       <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -885,10 +928,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:P38"/>
+  <dimension ref="A1:P40"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="B40" sqref="B40"/>
+      <selection activeCell="C41" sqref="C41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1342,6 +1385,28 @@
         <v>127</v>
       </c>
     </row>
+    <row r="39" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B39" s="11" t="s">
+        <v>128</v>
+      </c>
+      <c r="C39" t="s">
+        <v>129</v>
+      </c>
+      <c r="D39" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="40" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B40" s="11" t="s">
+        <v>130</v>
+      </c>
+      <c r="C40" s="15" t="s">
+        <v>131</v>
+      </c>
+      <c r="D40" t="s">
+        <v>127</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -1352,7 +1417,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:C81"/>
   <sheetViews>
-    <sheetView topLeftCell="A64" workbookViewId="0">
+    <sheetView topLeftCell="A52" workbookViewId="0">
       <selection activeCell="C83" sqref="C83"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
CARLA-5 pre-final DD and DPE from Tracy
</commit_message>
<xml_diff>
--- a/analyst/Tracy/rmonize/data_dictionary/DD_CARLA_TRACY.xlsx
+++ b/analyst/Tracy/rmonize/data_dictionary/DD_CARLA_TRACY.xlsx
@@ -1,27 +1,32 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="20417"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27932"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="K:\use-cases-harmonisation\use-cases-harmonisation\analyst\Tracy\rmonize\data_dictionary\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\schwarz-f\Desktop\use-cases-harmonisation\analyst\Tracy\rmonize\data_dictionary\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D2ED5B10-F0A0-4A12-BBBA-E831CC763ACA}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{244EC650-76B5-44AC-B125-56521A45E478}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Variables" sheetId="1" r:id="rId1"/>
     <sheet name="Categories" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xlwcv="http://schemas.microsoft.com/office/spreadsheetml/2024/workbookCompatibilityVersion" uri="{D14903EA-33C4-47F7-8F05-3474C54BE107}">
+      <xlwcv:version setVersion="1"/>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="282" uniqueCount="132">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="279" uniqueCount="128">
   <si>
     <t>index</t>
   </si>
@@ -38,9 +43,6 @@
     <t>variable</t>
   </si>
   <si>
-    <t>ID</t>
-  </si>
-  <si>
     <t>integer</t>
   </si>
   <si>
@@ -59,9 +61,6 @@
     <t>work_status</t>
   </si>
   <si>
-    <t xml:space="preserve"> employ</t>
-  </si>
-  <si>
     <t>Current status of occupation</t>
   </si>
   <si>
@@ -224,9 +223,6 @@
     <t>poss. by MI_final/CABG/PTCA/stroke/carotis-OP</t>
   </si>
   <si>
-    <t xml:space="preserve"> yes</t>
-  </si>
-  <si>
     <t>Yes</t>
   </si>
   <si>
@@ -257,9 +253,6 @@
     <t>No/don't know</t>
   </si>
   <si>
-    <t>don't know</t>
-  </si>
-  <si>
     <t>student</t>
   </si>
   <si>
@@ -326,21 +319,12 @@
     <t xml:space="preserve">ID </t>
   </si>
   <si>
-    <t>MED_STAT</t>
-  </si>
-  <si>
-    <t>MED_NSAID</t>
-  </si>
-  <si>
     <t>Regular use of statins</t>
   </si>
   <si>
     <t>Regular use of non-steroidal anti-inflammatory drugs</t>
   </si>
   <si>
-    <t xml:space="preserve">f1_htn_kora </t>
-  </si>
-  <si>
     <t>f2_htn_kora</t>
   </si>
   <si>
@@ -374,12 +358,6 @@
     <t>Currently nr. smoked cigars/day</t>
   </si>
   <si>
-    <t>AGE_HYP</t>
-  </si>
-  <si>
-    <t>Age at diagnosis of essential hypertension</t>
-  </si>
-  <si>
     <t xml:space="preserve">no </t>
   </si>
   <si>
@@ -407,47 +385,38 @@
     <t>date</t>
   </si>
   <si>
-    <r>
-      <t>F1_untdat</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-  </si>
-  <si>
     <t>baseline examination for follow-up 1</t>
   </si>
   <si>
-    <r>
-      <t>F2_untdat</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-  </si>
-  <si>
     <t>baseline examination for follow-up 2</t>
+  </si>
+  <si>
+    <t>employ</t>
+  </si>
+  <si>
+    <t>f1_htn_kora</t>
+  </si>
+  <si>
+    <t>id</t>
+  </si>
+  <si>
+    <t>med_stat</t>
+  </si>
+  <si>
+    <t>med_nsaid</t>
+  </si>
+  <si>
+    <t xml:space="preserve">f1_untdat </t>
+  </si>
+  <si>
+    <t xml:space="preserve">f2_untdat </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -494,13 +463,6 @@
       <i/>
       <sz val="11"/>
       <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -592,7 +554,7 @@
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
@@ -608,9 +570,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2007 - 2010">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -648,9 +610,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2007 - 2010">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -683,26 +645,9 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -735,26 +680,9 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2007 - 2010">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -928,13 +856,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:P40"/>
+  <dimension ref="A1:P39"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="C41" sqref="C41"/>
+    <sheetView topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="B40" sqref="B40"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="18.140625" style="11" customWidth="1"/>
     <col min="3" max="3" width="59.28515625" style="11" bestFit="1" customWidth="1"/>
@@ -956,455 +884,444 @@
     </row>
     <row r="2" spans="1:4" s="6" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B2" s="23" t="s">
-        <v>5</v>
+        <v>123</v>
       </c>
       <c r="C2" s="18" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="D2" s="18" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B3" s="3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B4" s="3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D4" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
     </row>
     <row r="5" spans="1:4" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B5" s="15" t="s">
+        <v>8</v>
+      </c>
+      <c r="C5" s="15" t="s">
         <v>9</v>
       </c>
-      <c r="C5" s="15" t="s">
-        <v>10</v>
-      </c>
       <c r="D5" s="6" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="6" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B6" s="15" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="C6" s="19" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="D6" s="6" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B7" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D7" t="s">
         <v>15</v>
-      </c>
-      <c r="C7" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="D7" t="s">
-        <v>17</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B8" s="5" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="D8" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B9" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="C9" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="C9" s="13" t="s">
-        <v>13</v>
-      </c>
       <c r="D9" s="6" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B10" s="13" t="s">
+        <v>121</v>
+      </c>
+      <c r="C10" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="C10" s="13" t="s">
-        <v>14</v>
-      </c>
       <c r="D10" s="6" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="11" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B11" s="3" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="D11" s="6" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
     </row>
     <row r="12" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B12" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="C12" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="C12" s="3" t="s">
-        <v>21</v>
-      </c>
       <c r="D12" s="6" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
     </row>
     <row r="13" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B13" s="16" t="s">
-        <v>115</v>
+        <v>108</v>
       </c>
       <c r="C13" s="19" t="s">
-        <v>116</v>
+        <v>109</v>
       </c>
       <c r="D13" s="6" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
     </row>
     <row r="14" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B14" s="19" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="C14" s="19" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="D14" s="6" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B15" s="3" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="D15" s="6" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B16" s="3" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="D16" s="6" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="17" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B17" s="19" t="s">
-        <v>111</v>
+        <v>104</v>
       </c>
       <c r="C17" s="19" t="s">
-        <v>113</v>
+        <v>106</v>
       </c>
       <c r="D17" s="6" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="18" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B18" s="16" t="s">
-        <v>112</v>
+        <v>105</v>
       </c>
       <c r="C18" s="19" t="s">
-        <v>114</v>
+        <v>107</v>
       </c>
       <c r="D18" s="6" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="19" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B19" s="3" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C19" s="3" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="D19" s="6" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="20" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B20" s="16" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="C20" s="3" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="D20" s="6" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="21" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B21" s="3" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C21" s="3" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="D21" s="6" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="22" spans="2:4" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B22" s="15" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C22" s="15" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="D22" s="6" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="23" spans="2:4" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B23" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="C23" s="15" t="s">
+        <v>28</v>
+      </c>
+      <c r="D23" s="6" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="24" spans="2:4" s="4" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="B24" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="C24" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="D24" s="6" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="25" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B25" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="C23" s="15" t="s">
-        <v>30</v>
-      </c>
-      <c r="D23" s="6" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="24" spans="2:4" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B24" s="6" t="s">
-        <v>117</v>
-      </c>
-      <c r="C24" s="18" t="s">
-        <v>118</v>
-      </c>
-      <c r="D24" s="6" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="25" spans="2:4" s="4" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="B25" s="3" t="s">
-        <v>32</v>
-      </c>
       <c r="C25" s="3" t="s">
-        <v>33</v>
+        <v>86</v>
       </c>
       <c r="D25" s="6" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="26" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B26" s="3" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="C26" s="3" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="D26" s="6" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="27" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B27" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C27" s="3" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="D27" s="6" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="28" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B28" s="3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C28" s="3" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="D28" s="6" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="29" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B29" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="C29" s="3" t="s">
-        <v>93</v>
+      <c r="B29" s="6" t="s">
+        <v>124</v>
+      </c>
+      <c r="C29" s="6" t="s">
+        <v>97</v>
       </c>
       <c r="D29" s="6" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="30" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B30" s="6" t="s">
-        <v>101</v>
+        <v>125</v>
       </c>
       <c r="C30" s="6" t="s">
-        <v>103</v>
+        <v>98</v>
       </c>
       <c r="D30" s="6" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="31" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B31" s="6" t="s">
-        <v>102</v>
-      </c>
-      <c r="C31" s="6" t="s">
-        <v>104</v>
+        <v>122</v>
+      </c>
+      <c r="C31" s="15" t="s">
+        <v>100</v>
       </c>
       <c r="D31" s="6" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="32" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B32" s="6" t="s">
-        <v>105</v>
+        <v>99</v>
       </c>
       <c r="C32" s="15" t="s">
-        <v>107</v>
+        <v>101</v>
       </c>
       <c r="D32" s="6" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="33" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B33" s="6" t="s">
-        <v>106</v>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="33" spans="2:16" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B33" s="15" t="s">
+        <v>35</v>
       </c>
       <c r="C33" s="15" t="s">
-        <v>108</v>
-      </c>
-      <c r="D33" s="6" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="34" spans="2:16" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+        <v>36</v>
+      </c>
+      <c r="D33" s="16" t="s">
+        <v>5</v>
+      </c>
+      <c r="E33" s="17"/>
+      <c r="F33" s="17"/>
+      <c r="G33" s="14"/>
+      <c r="H33" s="14"/>
+      <c r="I33" s="14"/>
+      <c r="J33" s="14"/>
+      <c r="K33" s="14"/>
+      <c r="L33" s="14"/>
+      <c r="M33" s="14"/>
+      <c r="N33" s="14"/>
+      <c r="O33" s="14"/>
+      <c r="P33" s="14"/>
+    </row>
+    <row r="34" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B34" s="15" t="s">
+        <v>103</v>
+      </c>
+      <c r="C34" s="7" t="s">
+        <v>111</v>
+      </c>
+      <c r="D34" s="5" t="s">
+        <v>118</v>
+      </c>
+      <c r="E34" s="5"/>
+      <c r="F34" s="5"/>
+      <c r="G34" s="5"/>
+      <c r="H34" s="5"/>
+      <c r="I34" s="5"/>
+      <c r="J34" s="5"/>
+      <c r="K34" s="5"/>
+      <c r="L34" s="5"/>
+      <c r="M34" s="5"/>
+      <c r="N34" s="5"/>
+      <c r="O34" s="5"/>
+      <c r="P34" s="5"/>
+    </row>
+    <row r="35" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B35" s="7" t="s">
         <v>37</v>
       </c>
-      <c r="C34" s="15" t="s">
-        <v>38</v>
-      </c>
-      <c r="D34" s="16" t="s">
-        <v>6</v>
-      </c>
-      <c r="E34" s="17"/>
-      <c r="F34" s="17"/>
-      <c r="G34" s="14"/>
-      <c r="H34" s="14"/>
-      <c r="I34" s="14"/>
-      <c r="J34" s="14"/>
-      <c r="K34" s="14"/>
-      <c r="L34" s="14"/>
-      <c r="M34" s="14"/>
-      <c r="N34" s="14"/>
-      <c r="O34" s="14"/>
-      <c r="P34" s="14"/>
-    </row>
-    <row r="35" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B35" s="15" t="s">
-        <v>110</v>
-      </c>
       <c r="C35" s="7" t="s">
-        <v>120</v>
-      </c>
-      <c r="D35" s="5" t="s">
-        <v>127</v>
-      </c>
-      <c r="E35" s="5"/>
-      <c r="F35" s="5"/>
-      <c r="G35" s="5"/>
-      <c r="H35" s="5"/>
-      <c r="I35" s="5"/>
-      <c r="J35" s="5"/>
-      <c r="K35" s="5"/>
-      <c r="L35" s="5"/>
-      <c r="M35" s="5"/>
-      <c r="N35" s="5"/>
-      <c r="O35" s="5"/>
-      <c r="P35" s="5"/>
+        <v>90</v>
+      </c>
+      <c r="D35" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="36" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B36" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="C36" s="7" t="s">
         <v>39</v>
       </c>
-      <c r="C36" s="7" t="s">
-        <v>94</v>
-      </c>
       <c r="D36" t="s">
-        <v>6</v>
+        <v>118</v>
       </c>
     </row>
     <row r="37" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B37" s="7" t="s">
-        <v>40</v>
-      </c>
-      <c r="C37" s="7" t="s">
-        <v>41</v>
+      <c r="B37" s="11" t="s">
+        <v>102</v>
+      </c>
+      <c r="C37" t="s">
+        <v>112</v>
       </c>
       <c r="D37" t="s">
-        <v>127</v>
+        <v>118</v>
       </c>
     </row>
     <row r="38" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B38" s="11" t="s">
-        <v>109</v>
+        <v>126</v>
       </c>
       <c r="C38" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="D38" t="s">
-        <v>127</v>
+        <v>118</v>
       </c>
     </row>
     <row r="39" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B39" s="11" t="s">
-        <v>128</v>
-      </c>
-      <c r="C39" t="s">
-        <v>129</v>
+        <v>127</v>
+      </c>
+      <c r="C39" s="15" t="s">
+        <v>120</v>
       </c>
       <c r="D39" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="40" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B40" s="11" t="s">
-        <v>130</v>
-      </c>
-      <c r="C40" s="15" t="s">
-        <v>131</v>
-      </c>
-      <c r="D40" t="s">
-        <v>127</v>
+        <v>118</v>
       </c>
     </row>
   </sheetData>
@@ -1417,11 +1334,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:C81"/>
   <sheetViews>
-    <sheetView topLeftCell="A52" workbookViewId="0">
-      <selection activeCell="C83" sqref="C83"/>
+    <sheetView tabSelected="1" topLeftCell="A45" workbookViewId="0">
+      <selection activeCell="C60" sqref="C60"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="17.7109375" customWidth="1"/>
     <col min="2" max="2" width="11.28515625" customWidth="1"/>
@@ -1441,871 +1358,871 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B2">
         <v>1</v>
       </c>
       <c r="C2" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B3">
         <v>2</v>
       </c>
       <c r="C3" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B4">
         <v>1</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="9" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B5">
         <v>2</v>
       </c>
       <c r="C5" s="19" t="s">
-        <v>126</v>
+        <v>117</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A6" s="9" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B6">
         <v>3</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
     </row>
     <row r="7" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A7" s="9" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B7">
         <v>4</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
     </row>
     <row r="8" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A8" s="9" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B8">
         <v>5</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
     </row>
     <row r="9" spans="1:3" ht="45" x14ac:dyDescent="0.25">
       <c r="A9" s="9" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B9">
         <v>6</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" s="9" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B10">
         <v>7</v>
       </c>
       <c r="C10" s="9" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" s="15" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="B11">
         <v>1</v>
       </c>
       <c r="C11" s="16" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" s="15" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="B12">
         <v>2</v>
       </c>
       <c r="C12" s="16" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" s="15" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="B13">
         <v>3</v>
       </c>
       <c r="C13" s="16" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" s="15" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="B14">
         <v>4</v>
       </c>
       <c r="C14" s="16" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" s="15" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="B15">
         <v>5</v>
       </c>
       <c r="C15" s="16" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
     </row>
     <row r="16" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A16" s="15" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="B16">
         <v>6</v>
       </c>
       <c r="C16" s="16" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" s="15" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="B17">
         <v>7</v>
       </c>
       <c r="C17" s="16" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" s="15" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="B18">
         <v>8</v>
       </c>
       <c r="C18" s="16" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" s="8" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B19">
         <v>1</v>
       </c>
       <c r="C19" s="9" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" s="8" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B20">
         <v>2</v>
       </c>
       <c r="C20" s="9" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" s="8" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B21">
         <v>3</v>
       </c>
       <c r="C21" s="9" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" s="13" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B22" s="6">
         <v>1</v>
       </c>
       <c r="C22" s="18" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" s="13" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B23" s="6">
         <v>2</v>
       </c>
       <c r="C23" s="18" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" s="13" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B24" s="6">
         <v>3</v>
       </c>
       <c r="C24" s="18" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" s="13" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B25" s="6">
         <v>4</v>
       </c>
       <c r="C25" s="18" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" s="13" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B26" s="6">
         <v>5</v>
       </c>
       <c r="C26" s="18" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" s="13" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B27" s="6">
         <v>6</v>
       </c>
       <c r="C27" s="18" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
     <row r="28" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A28" s="13" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B28" s="6">
         <v>7</v>
       </c>
       <c r="C28" s="18" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" s="13" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B29" s="6">
         <v>8</v>
       </c>
       <c r="C29" s="18" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" s="13" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B30" s="6">
         <v>9</v>
       </c>
       <c r="C30" s="18" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" s="13" t="s">
-        <v>12</v>
+        <v>121</v>
       </c>
       <c r="B31" s="6">
         <v>1</v>
       </c>
       <c r="C31" s="18" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32" s="13" t="s">
-        <v>12</v>
+        <v>121</v>
       </c>
       <c r="B32" s="6">
         <v>2</v>
       </c>
       <c r="C32" s="18" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" s="13" t="s">
-        <v>12</v>
+        <v>121</v>
       </c>
       <c r="B33" s="6">
         <v>3</v>
       </c>
       <c r="C33" s="18" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34" s="13" t="s">
-        <v>12</v>
+        <v>121</v>
       </c>
       <c r="B34" s="6">
         <v>4</v>
       </c>
       <c r="C34" s="18" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35" s="15" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B35" s="20">
         <v>0</v>
       </c>
       <c r="C35" s="16" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A36" s="15" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B36" s="20">
         <v>1</v>
       </c>
       <c r="C36" s="16" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
     </row>
     <row r="37" spans="1:3" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A37" s="6" t="s">
-        <v>111</v>
+        <v>104</v>
       </c>
       <c r="B37" s="24">
         <v>1</v>
       </c>
       <c r="C37" s="24" t="s">
-        <v>122</v>
+        <v>113</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A38" s="19" t="s">
-        <v>111</v>
+        <v>104</v>
       </c>
       <c r="B38" s="24">
         <v>2</v>
       </c>
       <c r="C38" s="24" t="s">
-        <v>123</v>
+        <v>114</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A39" s="19" t="s">
-        <v>111</v>
+        <v>104</v>
       </c>
       <c r="B39" s="24">
         <v>3</v>
       </c>
       <c r="C39" s="24" t="s">
-        <v>119</v>
+        <v>110</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A40" s="16" t="s">
-        <v>112</v>
+        <v>105</v>
       </c>
       <c r="B40" s="24">
         <v>1</v>
       </c>
       <c r="C40" s="24" t="s">
-        <v>124</v>
+        <v>115</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A41" s="16" t="s">
-        <v>112</v>
+        <v>105</v>
       </c>
       <c r="B41" s="24">
         <v>2</v>
       </c>
       <c r="C41" s="24" t="s">
-        <v>125</v>
+        <v>116</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A42" s="16" t="s">
-        <v>112</v>
+        <v>105</v>
       </c>
       <c r="B42" s="6">
         <v>3</v>
       </c>
       <c r="C42" s="6" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A43" s="10" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B43">
         <v>1</v>
       </c>
       <c r="C43" s="9" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A44" s="10" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B44">
         <v>2</v>
       </c>
       <c r="C44" s="9" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A45" s="10" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B45">
         <v>9</v>
       </c>
       <c r="C45" s="9" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A46" s="9" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B46">
         <v>0</v>
       </c>
       <c r="C46" s="9" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A47" s="9" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B47">
         <v>1</v>
       </c>
       <c r="C47" s="9" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A48" s="15" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B48" s="22">
         <v>1</v>
       </c>
       <c r="C48" s="15" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A49" s="15" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B49" s="22">
         <v>2</v>
       </c>
       <c r="C49" s="15" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A50" s="15" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B50" s="20">
         <v>0</v>
       </c>
       <c r="C50" s="16" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A51" s="15" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B51" s="20">
         <v>1</v>
       </c>
       <c r="C51" s="16" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A52" s="10" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B52">
         <v>0</v>
       </c>
       <c r="C52" s="16" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A53" s="10" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B53">
         <v>1</v>
       </c>
       <c r="C53" s="9" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
     </row>
     <row r="54" spans="1:3" ht="45" x14ac:dyDescent="0.25">
       <c r="A54" s="10" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B54">
         <v>2</v>
       </c>
       <c r="C54" s="9" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A55" s="9" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B55">
         <v>0</v>
       </c>
       <c r="C55" s="9" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A56" s="9" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B56">
         <v>1</v>
       </c>
       <c r="C56" s="9" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A57" s="9" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B57">
         <v>1</v>
       </c>
       <c r="C57" s="9" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A58" s="9" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B58">
         <v>2</v>
       </c>
       <c r="C58" s="9" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A59" s="9" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B59">
         <v>3</v>
       </c>
       <c r="C59" s="9" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A60" s="9" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B60">
         <v>8</v>
       </c>
       <c r="C60" s="9" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A61" s="9" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B61">
         <v>1</v>
       </c>
       <c r="C61" s="9" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A62" s="9" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B62">
         <v>2</v>
       </c>
       <c r="C62" s="9" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A63" s="9" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B63">
         <v>3</v>
       </c>
       <c r="C63" s="9" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A64" s="9" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B64">
         <v>8</v>
       </c>
       <c r="C64" s="9" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A65" s="9" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B65">
         <v>1</v>
       </c>
       <c r="C65" s="9" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A66" s="9" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B66">
         <v>2</v>
       </c>
       <c r="C66" s="9" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A67" s="9" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B67">
         <v>3</v>
       </c>
       <c r="C67" s="9" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A68" s="9" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B68">
         <v>8</v>
       </c>
       <c r="C68" s="9" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A69" s="6" t="s">
-        <v>101</v>
+        <v>124</v>
       </c>
       <c r="B69" s="22">
         <v>0</v>
       </c>
       <c r="C69" s="15" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A70" s="6" t="s">
-        <v>101</v>
+        <v>124</v>
       </c>
       <c r="B70" s="22">
         <v>1</v>
       </c>
       <c r="C70" s="15" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A71" s="6" t="s">
-        <v>102</v>
+        <v>125</v>
       </c>
       <c r="B71" s="22">
         <v>0</v>
       </c>
       <c r="C71" s="15" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
     </row>
     <row r="72" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A72" s="6" t="s">
-        <v>102</v>
+        <v>125</v>
       </c>
       <c r="B72" s="22">
         <v>1</v>
       </c>
       <c r="C72" s="15" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
     </row>
     <row r="73" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A73" s="6" t="s">
-        <v>105</v>
+        <v>122</v>
       </c>
       <c r="B73" s="20">
         <v>0</v>
       </c>
       <c r="C73" s="16" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
     </row>
     <row r="74" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A74" s="6" t="s">
-        <v>105</v>
+        <v>122</v>
       </c>
       <c r="B74" s="20">
         <v>1</v>
       </c>
       <c r="C74" s="16" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
     </row>
     <row r="75" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A75" s="6" t="s">
-        <v>106</v>
+        <v>99</v>
       </c>
       <c r="B75" s="20">
         <v>0</v>
       </c>
       <c r="C75" s="16" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
     </row>
     <row r="76" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A76" s="6" t="s">
-        <v>106</v>
+        <v>99</v>
       </c>
       <c r="B76" s="20">
         <v>1</v>
       </c>
       <c r="C76" s="16" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
     </row>
     <row r="77" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B77">
         <v>0</v>
       </c>
       <c r="C77" s="12" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
     </row>
     <row r="78" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B78">
         <v>1</v>
       </c>
       <c r="C78" s="12" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
     </row>
     <row r="79" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A79" s="15" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B79" s="20">
         <v>0</v>
       </c>
       <c r="C79" s="16" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
     </row>
     <row r="80" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A80" s="15" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B80" s="20">
         <v>1</v>
       </c>
       <c r="C80" s="16" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
     </row>
     <row r="81" spans="2:2" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
adjusted DD and DPE documents for CARLA; open question AGE_FUP
</commit_message>
<xml_diff>
--- a/analyst/Tracy/rmonize/data_dictionary/DD_CARLA_TRACY.xlsx
+++ b/analyst/Tracy/rmonize/data_dictionary/DD_CARLA_TRACY.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\schwarz-f\Desktop\use-cases-harmonisation\analyst\Tracy\rmonize\data_dictionary\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{244EC650-76B5-44AC-B125-56521A45E478}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{86FC02DA-F831-4A12-9453-961A546D13F7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Variables" sheetId="1" r:id="rId1"/>
@@ -858,8 +858,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:P39"/>
   <sheetViews>
-    <sheetView topLeftCell="A9" workbookViewId="0">
-      <selection activeCell="B40" sqref="B40"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1334,7 +1334,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:C81"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A45" workbookViewId="0">
+    <sheetView topLeftCell="A45" workbookViewId="0">
       <selection activeCell="C60" sqref="C60"/>
     </sheetView>
   </sheetViews>

</xml_diff>